<commit_message>
Modificaciones en certificado de aceptación y archivo modelo
</commit_message>
<xml_diff>
--- a/public/file_layouts/OC_Certificate_model.xlsx
+++ b/public/file_layouts/OC_Certificate_model.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cite\public\file_layouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\services\public\file_layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EB7C78CE-7A02-4AF4-8B9E-F134D3FEBFD4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="253"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="253" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certificado" sheetId="8" r:id="rId1"/>
@@ -73,9 +74,6 @@
     </r>
   </si>
   <si>
-    <t>Pza</t>
-  </si>
-  <si>
     <t>00/100 Bolivianos</t>
   </si>
   <si>
@@ -133,9 +131,6 @@
     <t>Código:</t>
   </si>
   <si>
-    <t>Historial de pagos</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -171,11 +166,17 @@
   <si>
     <t>IV. AUTORIZACIÓN</t>
   </si>
+  <si>
+    <t>Glb</t>
+  </si>
+  <si>
+    <t>Historial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -637,269 +638,269 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规_Quotation for Civil Works(按年度含SA1104)" xfId="2"/>
+    <cellStyle name="常规_Quotation for Civil Works(按年度含SA1104)" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -936,7 +937,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6230" name="3 Imagen"/>
+        <xdr:cNvPr id="6230" name="3 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056180000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1046,6 +1053,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1081,6 +1105,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1256,14 +1297,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AX73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AW56" sqref="AW56"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AW14" sqref="AW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1350,7 +1391,7 @@
       </c>
       <c r="AS1" s="7"/>
       <c r="AT1" s="59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AU1" s="9"/>
       <c r="AV1" s="14"/>
@@ -1381,7 +1422,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
@@ -1396,10 +1437,10 @@
       <c r="AJ2" s="4"/>
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
-      <c r="AM2" s="128"/>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="128"/>
-      <c r="AP2" s="128"/>
+      <c r="AM2" s="156"/>
+      <c r="AN2" s="156"/>
+      <c r="AO2" s="156"/>
+      <c r="AP2" s="156"/>
       <c r="AQ2" s="22"/>
       <c r="AR2" s="4"/>
       <c r="AS2" s="4"/>
@@ -1602,13 +1643,13 @@
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
-      <c r="AM6" s="129"/>
-      <c r="AN6" s="129"/>
-      <c r="AO6" s="129"/>
-      <c r="AP6" s="129"/>
-      <c r="AQ6" s="129"/>
-      <c r="AR6" s="129"/>
-      <c r="AS6" s="129"/>
+      <c r="AM6" s="157"/>
+      <c r="AN6" s="157"/>
+      <c r="AO6" s="157"/>
+      <c r="AP6" s="157"/>
+      <c r="AQ6" s="157"/>
+      <c r="AR6" s="157"/>
+      <c r="AS6" s="157"/>
       <c r="AT6" s="22"/>
       <c r="AU6" s="23"/>
       <c r="AV6" s="14"/>
@@ -1646,7 +1687,7 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
@@ -1766,55 +1807,55 @@
       <c r="AV9" s="14"/>
     </row>
     <row r="10" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="146" t="s">
-        <v>15</v>
+      <c r="A10" s="122" t="s">
+        <v>14</v>
       </c>
-      <c r="B10" s="147"/>
-      <c r="C10" s="147"/>
-      <c r="D10" s="147"/>
-      <c r="E10" s="147"/>
-      <c r="F10" s="147"/>
-      <c r="G10" s="147"/>
-      <c r="H10" s="147"/>
-      <c r="I10" s="147"/>
-      <c r="J10" s="147"/>
-      <c r="K10" s="147"/>
-      <c r="L10" s="147"/>
-      <c r="M10" s="147"/>
-      <c r="N10" s="147"/>
-      <c r="O10" s="147"/>
-      <c r="P10" s="147"/>
-      <c r="Q10" s="147"/>
-      <c r="R10" s="147"/>
-      <c r="S10" s="147"/>
-      <c r="T10" s="147"/>
-      <c r="U10" s="147"/>
-      <c r="V10" s="147"/>
-      <c r="W10" s="147"/>
-      <c r="X10" s="147"/>
-      <c r="Y10" s="147"/>
-      <c r="Z10" s="147"/>
-      <c r="AA10" s="147"/>
-      <c r="AB10" s="147"/>
-      <c r="AC10" s="147"/>
-      <c r="AD10" s="147"/>
-      <c r="AE10" s="147"/>
-      <c r="AF10" s="147"/>
-      <c r="AG10" s="147"/>
-      <c r="AH10" s="147"/>
-      <c r="AI10" s="147"/>
-      <c r="AJ10" s="147"/>
-      <c r="AK10" s="147"/>
-      <c r="AL10" s="147"/>
-      <c r="AM10" s="147"/>
-      <c r="AN10" s="147"/>
-      <c r="AO10" s="147"/>
-      <c r="AP10" s="147"/>
-      <c r="AQ10" s="147"/>
-      <c r="AR10" s="147"/>
-      <c r="AS10" s="147"/>
-      <c r="AT10" s="147"/>
-      <c r="AU10" s="148"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="123"/>
+      <c r="N10" s="123"/>
+      <c r="O10" s="123"/>
+      <c r="P10" s="123"/>
+      <c r="Q10" s="123"/>
+      <c r="R10" s="123"/>
+      <c r="S10" s="123"/>
+      <c r="T10" s="123"/>
+      <c r="U10" s="123"/>
+      <c r="V10" s="123"/>
+      <c r="W10" s="123"/>
+      <c r="X10" s="123"/>
+      <c r="Y10" s="123"/>
+      <c r="Z10" s="123"/>
+      <c r="AA10" s="123"/>
+      <c r="AB10" s="123"/>
+      <c r="AC10" s="123"/>
+      <c r="AD10" s="123"/>
+      <c r="AE10" s="123"/>
+      <c r="AF10" s="123"/>
+      <c r="AG10" s="123"/>
+      <c r="AH10" s="123"/>
+      <c r="AI10" s="123"/>
+      <c r="AJ10" s="123"/>
+      <c r="AK10" s="123"/>
+      <c r="AL10" s="123"/>
+      <c r="AM10" s="123"/>
+      <c r="AN10" s="123"/>
+      <c r="AO10" s="123"/>
+      <c r="AP10" s="123"/>
+      <c r="AQ10" s="123"/>
+      <c r="AR10" s="123"/>
+      <c r="AS10" s="123"/>
+      <c r="AT10" s="123"/>
+      <c r="AU10" s="124"/>
       <c r="AV10" s="14"/>
     </row>
     <row r="11" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,7 +1910,7 @@
     </row>
     <row r="12" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1946,36 +1987,36 @@
       <c r="V13" s="16"/>
       <c r="W13" s="19"/>
       <c r="X13" s="16"/>
-      <c r="Y13" s="156"/>
-      <c r="Z13" s="156"/>
-      <c r="AA13" s="156"/>
-      <c r="AB13" s="156"/>
-      <c r="AC13" s="156"/>
-      <c r="AD13" s="156"/>
-      <c r="AE13" s="156"/>
+      <c r="Y13" s="147"/>
+      <c r="Z13" s="147"/>
+      <c r="AA13" s="147"/>
+      <c r="AB13" s="147"/>
+      <c r="AC13" s="147"/>
+      <c r="AD13" s="147"/>
+      <c r="AE13" s="147"/>
       <c r="AF13" s="46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AG13" s="20"/>
       <c r="AH13" s="15"/>
       <c r="AI13" s="15"/>
       <c r="AJ13" s="15"/>
       <c r="AK13" s="15"/>
-      <c r="AL13" s="162"/>
-      <c r="AM13" s="162"/>
-      <c r="AN13" s="162"/>
-      <c r="AO13" s="162"/>
-      <c r="AP13" s="162"/>
-      <c r="AQ13" s="162"/>
-      <c r="AR13" s="162"/>
-      <c r="AS13" s="162"/>
-      <c r="AT13" s="162"/>
+      <c r="AL13" s="155"/>
+      <c r="AM13" s="155"/>
+      <c r="AN13" s="155"/>
+      <c r="AO13" s="155"/>
+      <c r="AP13" s="155"/>
+      <c r="AQ13" s="155"/>
+      <c r="AR13" s="155"/>
+      <c r="AS13" s="155"/>
+      <c r="AT13" s="155"/>
       <c r="AU13" s="27"/>
       <c r="AV13" s="14"/>
     </row>
     <row r="14" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -2008,7 +2049,7 @@
       <c r="AD14" s="15"/>
       <c r="AE14" s="15"/>
       <c r="AF14" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AG14" s="38"/>
       <c r="AH14" s="15"/>
@@ -2041,41 +2082,41 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="161"/>
-      <c r="M15" s="161"/>
-      <c r="N15" s="161"/>
-      <c r="O15" s="161"/>
-      <c r="P15" s="161"/>
-      <c r="Q15" s="161"/>
-      <c r="R15" s="161"/>
-      <c r="S15" s="161"/>
-      <c r="T15" s="161"/>
-      <c r="U15" s="161"/>
-      <c r="V15" s="161"/>
-      <c r="W15" s="161"/>
-      <c r="X15" s="161"/>
-      <c r="Y15" s="161"/>
-      <c r="Z15" s="161"/>
-      <c r="AA15" s="161"/>
-      <c r="AB15" s="161"/>
-      <c r="AC15" s="161"/>
-      <c r="AD15" s="161"/>
-      <c r="AE15" s="161"/>
-      <c r="AF15" s="161"/>
-      <c r="AG15" s="161"/>
-      <c r="AH15" s="161"/>
-      <c r="AI15" s="161"/>
-      <c r="AJ15" s="161"/>
-      <c r="AK15" s="161"/>
-      <c r="AL15" s="161"/>
-      <c r="AM15" s="161"/>
-      <c r="AN15" s="161"/>
-      <c r="AO15" s="161"/>
-      <c r="AP15" s="161"/>
-      <c r="AQ15" s="161"/>
-      <c r="AR15" s="161"/>
-      <c r="AS15" s="161"/>
-      <c r="AT15" s="161"/>
+      <c r="L15" s="154"/>
+      <c r="M15" s="154"/>
+      <c r="N15" s="154"/>
+      <c r="O15" s="154"/>
+      <c r="P15" s="154"/>
+      <c r="Q15" s="154"/>
+      <c r="R15" s="154"/>
+      <c r="S15" s="154"/>
+      <c r="T15" s="154"/>
+      <c r="U15" s="154"/>
+      <c r="V15" s="154"/>
+      <c r="W15" s="154"/>
+      <c r="X15" s="154"/>
+      <c r="Y15" s="154"/>
+      <c r="Z15" s="154"/>
+      <c r="AA15" s="154"/>
+      <c r="AB15" s="154"/>
+      <c r="AC15" s="154"/>
+      <c r="AD15" s="154"/>
+      <c r="AE15" s="154"/>
+      <c r="AF15" s="154"/>
+      <c r="AG15" s="154"/>
+      <c r="AH15" s="154"/>
+      <c r="AI15" s="154"/>
+      <c r="AJ15" s="154"/>
+      <c r="AK15" s="154"/>
+      <c r="AL15" s="154"/>
+      <c r="AM15" s="154"/>
+      <c r="AN15" s="154"/>
+      <c r="AO15" s="154"/>
+      <c r="AP15" s="154"/>
+      <c r="AQ15" s="154"/>
+      <c r="AR15" s="154"/>
+      <c r="AS15" s="154"/>
+      <c r="AT15" s="154"/>
       <c r="AU15" s="10"/>
       <c r="AV15" s="14"/>
     </row>
@@ -2130,55 +2171,55 @@
       <c r="AV16" s="14"/>
     </row>
     <row r="17" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="146" t="s">
-        <v>18</v>
+      <c r="A17" s="122" t="s">
+        <v>17</v>
       </c>
-      <c r="B17" s="147"/>
-      <c r="C17" s="147"/>
-      <c r="D17" s="147"/>
-      <c r="E17" s="147"/>
-      <c r="F17" s="147"/>
-      <c r="G17" s="147"/>
-      <c r="H17" s="147"/>
-      <c r="I17" s="147"/>
-      <c r="J17" s="147"/>
-      <c r="K17" s="147"/>
-      <c r="L17" s="147"/>
-      <c r="M17" s="147"/>
-      <c r="N17" s="147"/>
-      <c r="O17" s="147"/>
-      <c r="P17" s="147"/>
-      <c r="Q17" s="147"/>
-      <c r="R17" s="147"/>
-      <c r="S17" s="147"/>
-      <c r="T17" s="147"/>
-      <c r="U17" s="147"/>
-      <c r="V17" s="147"/>
-      <c r="W17" s="147"/>
-      <c r="X17" s="147"/>
-      <c r="Y17" s="147"/>
-      <c r="Z17" s="147"/>
-      <c r="AA17" s="147"/>
-      <c r="AB17" s="147"/>
-      <c r="AC17" s="147"/>
-      <c r="AD17" s="147"/>
-      <c r="AE17" s="147"/>
-      <c r="AF17" s="147"/>
-      <c r="AG17" s="147"/>
-      <c r="AH17" s="147"/>
-      <c r="AI17" s="147"/>
-      <c r="AJ17" s="147"/>
-      <c r="AK17" s="147"/>
-      <c r="AL17" s="147"/>
-      <c r="AM17" s="147"/>
-      <c r="AN17" s="147"/>
-      <c r="AO17" s="147"/>
-      <c r="AP17" s="147"/>
-      <c r="AQ17" s="147"/>
-      <c r="AR17" s="147"/>
-      <c r="AS17" s="147"/>
-      <c r="AT17" s="147"/>
-      <c r="AU17" s="148"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="123"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="123"/>
+      <c r="I17" s="123"/>
+      <c r="J17" s="123"/>
+      <c r="K17" s="123"/>
+      <c r="L17" s="123"/>
+      <c r="M17" s="123"/>
+      <c r="N17" s="123"/>
+      <c r="O17" s="123"/>
+      <c r="P17" s="123"/>
+      <c r="Q17" s="123"/>
+      <c r="R17" s="123"/>
+      <c r="S17" s="123"/>
+      <c r="T17" s="123"/>
+      <c r="U17" s="123"/>
+      <c r="V17" s="123"/>
+      <c r="W17" s="123"/>
+      <c r="X17" s="123"/>
+      <c r="Y17" s="123"/>
+      <c r="Z17" s="123"/>
+      <c r="AA17" s="123"/>
+      <c r="AB17" s="123"/>
+      <c r="AC17" s="123"/>
+      <c r="AD17" s="123"/>
+      <c r="AE17" s="123"/>
+      <c r="AF17" s="123"/>
+      <c r="AG17" s="123"/>
+      <c r="AH17" s="123"/>
+      <c r="AI17" s="123"/>
+      <c r="AJ17" s="123"/>
+      <c r="AK17" s="123"/>
+      <c r="AL17" s="123"/>
+      <c r="AM17" s="123"/>
+      <c r="AN17" s="123"/>
+      <c r="AO17" s="123"/>
+      <c r="AP17" s="123"/>
+      <c r="AQ17" s="123"/>
+      <c r="AR17" s="123"/>
+      <c r="AS17" s="123"/>
+      <c r="AT17" s="123"/>
+      <c r="AU17" s="124"/>
       <c r="AV17" s="14"/>
     </row>
     <row r="18" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2233,7 +2274,7 @@
     </row>
     <row r="19" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2246,7 +2287,7 @@
       <c r="J19" s="47"/>
       <c r="K19" s="4"/>
       <c r="L19" s="47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" s="75"/>
       <c r="N19" s="4"/>
@@ -2255,7 +2296,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="47"/>
       <c r="S19" s="47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="76"/>
@@ -2266,7 +2307,7 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
       <c r="AB19" s="47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
@@ -2341,7 +2382,7 @@
     </row>
     <row r="21" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="62"/>
       <c r="C21" s="62"/>
@@ -2356,7 +2397,7 @@
       <c r="L21" s="62"/>
       <c r="M21" s="70"/>
       <c r="N21" s="61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O21" s="62"/>
       <c r="P21" s="70"/>
@@ -2370,7 +2411,7 @@
       <c r="X21" s="70"/>
       <c r="Y21" s="70"/>
       <c r="Z21" s="61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AA21" s="70"/>
       <c r="AB21" s="62"/>
@@ -2380,7 +2421,7 @@
       <c r="AF21" s="70"/>
       <c r="AG21" s="70"/>
       <c r="AH21" s="61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AI21" s="70"/>
       <c r="AJ21" s="62"/>
@@ -2398,39 +2439,39 @@
       <c r="AV21" s="14"/>
     </row>
     <row r="22" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="115"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="166"/>
-      <c r="D22" s="166"/>
-      <c r="E22" s="166"/>
-      <c r="F22" s="166"/>
-      <c r="G22" s="166"/>
-      <c r="H22" s="166"/>
-      <c r="I22" s="166"/>
-      <c r="J22" s="166"/>
-      <c r="K22" s="166"/>
-      <c r="L22" s="166"/>
-      <c r="M22" s="116"/>
-      <c r="N22" s="167"/>
-      <c r="O22" s="168"/>
-      <c r="P22" s="168"/>
-      <c r="Q22" s="168"/>
-      <c r="R22" s="168"/>
-      <c r="S22" s="168"/>
-      <c r="T22" s="168"/>
-      <c r="U22" s="168"/>
-      <c r="V22" s="168"/>
-      <c r="W22" s="168"/>
-      <c r="X22" s="168"/>
-      <c r="Y22" s="169"/>
-      <c r="Z22" s="167"/>
-      <c r="AA22" s="168"/>
-      <c r="AB22" s="168"/>
-      <c r="AC22" s="168"/>
-      <c r="AD22" s="168"/>
-      <c r="AE22" s="168"/>
-      <c r="AF22" s="168"/>
-      <c r="AG22" s="169"/>
+      <c r="A22" s="116"/>
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="117"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="117"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="120"/>
+      <c r="P22" s="120"/>
+      <c r="Q22" s="120"/>
+      <c r="R22" s="120"/>
+      <c r="S22" s="120"/>
+      <c r="T22" s="120"/>
+      <c r="U22" s="120"/>
+      <c r="V22" s="120"/>
+      <c r="W22" s="120"/>
+      <c r="X22" s="120"/>
+      <c r="Y22" s="121"/>
+      <c r="Z22" s="119"/>
+      <c r="AA22" s="120"/>
+      <c r="AB22" s="120"/>
+      <c r="AC22" s="120"/>
+      <c r="AD22" s="120"/>
+      <c r="AE22" s="120"/>
+      <c r="AF22" s="120"/>
+      <c r="AG22" s="121"/>
       <c r="AH22" s="60"/>
       <c r="AI22" s="16"/>
       <c r="AJ22" s="16"/>
@@ -2498,113 +2539,113 @@
       <c r="AV23" s="14"/>
     </row>
     <row r="24" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="152" t="s">
+      <c r="A24" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="153"/>
-      <c r="C24" s="152" t="s">
-        <v>26</v>
+      <c r="B24" s="127"/>
+      <c r="C24" s="125" t="s">
+        <v>25</v>
       </c>
-      <c r="D24" s="170"/>
-      <c r="E24" s="170"/>
-      <c r="F24" s="170"/>
-      <c r="G24" s="170"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="170"/>
-      <c r="K24" s="170"/>
-      <c r="L24" s="170"/>
-      <c r="M24" s="170"/>
-      <c r="N24" s="170"/>
-      <c r="O24" s="170"/>
-      <c r="P24" s="170"/>
-      <c r="Q24" s="170"/>
-      <c r="R24" s="170"/>
-      <c r="S24" s="170"/>
-      <c r="T24" s="170"/>
-      <c r="U24" s="170"/>
-      <c r="V24" s="170"/>
-      <c r="W24" s="170"/>
-      <c r="X24" s="170"/>
-      <c r="Y24" s="170"/>
-      <c r="Z24" s="170"/>
-      <c r="AA24" s="170"/>
-      <c r="AB24" s="170"/>
-      <c r="AC24" s="170"/>
-      <c r="AD24" s="170"/>
-      <c r="AE24" s="153"/>
-      <c r="AF24" s="134" t="s">
+      <c r="D24" s="126"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="126"/>
+      <c r="G24" s="126"/>
+      <c r="H24" s="126"/>
+      <c r="I24" s="126"/>
+      <c r="J24" s="126"/>
+      <c r="K24" s="126"/>
+      <c r="L24" s="126"/>
+      <c r="M24" s="126"/>
+      <c r="N24" s="126"/>
+      <c r="O24" s="126"/>
+      <c r="P24" s="126"/>
+      <c r="Q24" s="126"/>
+      <c r="R24" s="126"/>
+      <c r="S24" s="126"/>
+      <c r="T24" s="126"/>
+      <c r="U24" s="126"/>
+      <c r="V24" s="126"/>
+      <c r="W24" s="126"/>
+      <c r="X24" s="126"/>
+      <c r="Y24" s="126"/>
+      <c r="Z24" s="126"/>
+      <c r="AA24" s="126"/>
+      <c r="AB24" s="126"/>
+      <c r="AC24" s="126"/>
+      <c r="AD24" s="126"/>
+      <c r="AE24" s="127"/>
+      <c r="AF24" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="AG24" s="135"/>
-      <c r="AH24" s="135"/>
-      <c r="AI24" s="136"/>
-      <c r="AJ24" s="134" t="s">
+      <c r="AG24" s="165"/>
+      <c r="AH24" s="165"/>
+      <c r="AI24" s="166"/>
+      <c r="AJ24" s="164" t="s">
         <v>1</v>
       </c>
-      <c r="AK24" s="135"/>
-      <c r="AL24" s="135"/>
-      <c r="AM24" s="136"/>
-      <c r="AN24" s="134" t="s">
-        <v>38</v>
+      <c r="AK24" s="165"/>
+      <c r="AL24" s="165"/>
+      <c r="AM24" s="166"/>
+      <c r="AN24" s="164" t="s">
+        <v>36</v>
       </c>
-      <c r="AO24" s="135"/>
-      <c r="AP24" s="135"/>
-      <c r="AQ24" s="135"/>
-      <c r="AR24" s="135"/>
-      <c r="AS24" s="135"/>
-      <c r="AT24" s="135"/>
-      <c r="AU24" s="136"/>
+      <c r="AO24" s="165"/>
+      <c r="AP24" s="165"/>
+      <c r="AQ24" s="165"/>
+      <c r="AR24" s="165"/>
+      <c r="AS24" s="165"/>
+      <c r="AT24" s="165"/>
+      <c r="AU24" s="166"/>
       <c r="AV24" s="14"/>
     </row>
     <row r="25" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="154"/>
-      <c r="B25" s="155"/>
-      <c r="C25" s="154"/>
-      <c r="D25" s="171"/>
-      <c r="E25" s="171"/>
-      <c r="F25" s="171"/>
-      <c r="G25" s="171"/>
-      <c r="H25" s="171"/>
-      <c r="I25" s="171"/>
-      <c r="J25" s="171"/>
-      <c r="K25" s="171"/>
-      <c r="L25" s="171"/>
-      <c r="M25" s="171"/>
-      <c r="N25" s="171"/>
-      <c r="O25" s="171"/>
-      <c r="P25" s="171"/>
-      <c r="Q25" s="171"/>
-      <c r="R25" s="171"/>
-      <c r="S25" s="171"/>
-      <c r="T25" s="171"/>
-      <c r="U25" s="171"/>
-      <c r="V25" s="171"/>
-      <c r="W25" s="171"/>
-      <c r="X25" s="171"/>
-      <c r="Y25" s="171"/>
-      <c r="Z25" s="171"/>
-      <c r="AA25" s="171"/>
-      <c r="AB25" s="171"/>
-      <c r="AC25" s="171"/>
-      <c r="AD25" s="171"/>
-      <c r="AE25" s="155"/>
-      <c r="AF25" s="137"/>
-      <c r="AG25" s="138"/>
-      <c r="AH25" s="138"/>
-      <c r="AI25" s="139"/>
-      <c r="AJ25" s="137"/>
-      <c r="AK25" s="138"/>
-      <c r="AL25" s="138"/>
-      <c r="AM25" s="139"/>
-      <c r="AN25" s="137"/>
-      <c r="AO25" s="138"/>
-      <c r="AP25" s="138"/>
-      <c r="AQ25" s="138"/>
-      <c r="AR25" s="138"/>
-      <c r="AS25" s="138"/>
-      <c r="AT25" s="138"/>
-      <c r="AU25" s="139"/>
+      <c r="A25" s="128"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="129"/>
+      <c r="E25" s="129"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="129"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="129"/>
+      <c r="J25" s="129"/>
+      <c r="K25" s="129"/>
+      <c r="L25" s="129"/>
+      <c r="M25" s="129"/>
+      <c r="N25" s="129"/>
+      <c r="O25" s="129"/>
+      <c r="P25" s="129"/>
+      <c r="Q25" s="129"/>
+      <c r="R25" s="129"/>
+      <c r="S25" s="129"/>
+      <c r="T25" s="129"/>
+      <c r="U25" s="129"/>
+      <c r="V25" s="129"/>
+      <c r="W25" s="129"/>
+      <c r="X25" s="129"/>
+      <c r="Y25" s="129"/>
+      <c r="Z25" s="129"/>
+      <c r="AA25" s="129"/>
+      <c r="AB25" s="129"/>
+      <c r="AC25" s="129"/>
+      <c r="AD25" s="129"/>
+      <c r="AE25" s="130"/>
+      <c r="AF25" s="167"/>
+      <c r="AG25" s="168"/>
+      <c r="AH25" s="168"/>
+      <c r="AI25" s="169"/>
+      <c r="AJ25" s="167"/>
+      <c r="AK25" s="168"/>
+      <c r="AL25" s="168"/>
+      <c r="AM25" s="169"/>
+      <c r="AN25" s="167"/>
+      <c r="AO25" s="168"/>
+      <c r="AP25" s="168"/>
+      <c r="AQ25" s="168"/>
+      <c r="AR25" s="168"/>
+      <c r="AS25" s="168"/>
+      <c r="AT25" s="168"/>
+      <c r="AU25" s="169"/>
       <c r="AV25" s="14"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.2">
@@ -2647,21 +2688,21 @@
       <c r="AK26" s="7"/>
       <c r="AL26" s="7"/>
       <c r="AM26" s="9"/>
-      <c r="AN26" s="172"/>
-      <c r="AO26" s="173"/>
-      <c r="AP26" s="173"/>
-      <c r="AQ26" s="173"/>
-      <c r="AR26" s="173"/>
-      <c r="AS26" s="173"/>
-      <c r="AT26" s="173"/>
-      <c r="AU26" s="174"/>
+      <c r="AN26" s="131"/>
+      <c r="AO26" s="132"/>
+      <c r="AP26" s="132"/>
+      <c r="AQ26" s="132"/>
+      <c r="AR26" s="132"/>
+      <c r="AS26" s="132"/>
+      <c r="AT26" s="132"/>
+      <c r="AU26" s="133"/>
       <c r="AV26" s="14"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A27" s="111">
+      <c r="A27" s="148">
         <v>1</v>
       </c>
-      <c r="B27" s="112"/>
+      <c r="B27" s="150"/>
       <c r="C27" s="44"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
@@ -2691,28 +2732,28 @@
       <c r="AC27" s="47"/>
       <c r="AD27" s="47"/>
       <c r="AE27" s="50"/>
-      <c r="AF27" s="140">
+      <c r="AF27" s="170">
         <v>1</v>
       </c>
-      <c r="AG27" s="141"/>
-      <c r="AH27" s="141"/>
-      <c r="AI27" s="142"/>
-      <c r="AJ27" s="111" t="s">
-        <v>11</v>
+      <c r="AG27" s="171"/>
+      <c r="AH27" s="171"/>
+      <c r="AI27" s="172"/>
+      <c r="AJ27" s="148" t="s">
+        <v>42</v>
       </c>
-      <c r="AK27" s="157"/>
-      <c r="AL27" s="157"/>
-      <c r="AM27" s="112"/>
-      <c r="AN27" s="149">
+      <c r="AK27" s="149"/>
+      <c r="AL27" s="149"/>
+      <c r="AM27" s="150"/>
+      <c r="AN27" s="176">
         <v>0</v>
       </c>
-      <c r="AO27" s="150"/>
-      <c r="AP27" s="150"/>
-      <c r="AQ27" s="150"/>
-      <c r="AR27" s="150"/>
-      <c r="AS27" s="150"/>
-      <c r="AT27" s="150"/>
-      <c r="AU27" s="151"/>
+      <c r="AO27" s="177"/>
+      <c r="AP27" s="177"/>
+      <c r="AQ27" s="177"/>
+      <c r="AR27" s="177"/>
+      <c r="AS27" s="177"/>
+      <c r="AT27" s="177"/>
+      <c r="AU27" s="178"/>
       <c r="AV27" s="14"/>
     </row>
     <row r="28" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
@@ -2747,141 +2788,141 @@
       <c r="AC28" s="49"/>
       <c r="AD28" s="49"/>
       <c r="AE28" s="85"/>
-      <c r="AF28" s="143"/>
-      <c r="AG28" s="144"/>
-      <c r="AH28" s="144"/>
-      <c r="AI28" s="145"/>
-      <c r="AJ28" s="158"/>
-      <c r="AK28" s="159"/>
-      <c r="AL28" s="159"/>
-      <c r="AM28" s="160"/>
-      <c r="AN28" s="175"/>
-      <c r="AO28" s="176"/>
-      <c r="AP28" s="176"/>
-      <c r="AQ28" s="176"/>
-      <c r="AR28" s="176"/>
-      <c r="AS28" s="176"/>
-      <c r="AT28" s="176"/>
-      <c r="AU28" s="177"/>
+      <c r="AF28" s="173"/>
+      <c r="AG28" s="174"/>
+      <c r="AH28" s="174"/>
+      <c r="AI28" s="175"/>
+      <c r="AJ28" s="151"/>
+      <c r="AK28" s="152"/>
+      <c r="AL28" s="152"/>
+      <c r="AM28" s="153"/>
+      <c r="AN28" s="134"/>
+      <c r="AO28" s="135"/>
+      <c r="AP28" s="135"/>
+      <c r="AQ28" s="135"/>
+      <c r="AR28" s="135"/>
+      <c r="AS28" s="135"/>
+      <c r="AT28" s="135"/>
+      <c r="AU28" s="136"/>
       <c r="AV28" s="74"/>
       <c r="AW28" s="51"/>
       <c r="AX28" s="51"/>
     </row>
     <row r="29" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="113" t="s">
-        <v>39</v>
+      <c r="A29" s="179" t="s">
+        <v>37</v>
       </c>
-      <c r="B29" s="114"/>
-      <c r="C29" s="120" t="s">
+      <c r="B29" s="180"/>
+      <c r="C29" s="181" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="182"/>
+      <c r="E29" s="182"/>
+      <c r="F29" s="182"/>
+      <c r="G29" s="182"/>
+      <c r="H29" s="182"/>
+      <c r="I29" s="182"/>
+      <c r="J29" s="182"/>
+      <c r="K29" s="182"/>
+      <c r="L29" s="182"/>
+      <c r="M29" s="182"/>
+      <c r="N29" s="182"/>
+      <c r="O29" s="182"/>
+      <c r="P29" s="182"/>
+      <c r="Q29" s="182"/>
+      <c r="R29" s="182"/>
+      <c r="S29" s="182"/>
+      <c r="T29" s="182"/>
+      <c r="U29" s="182"/>
+      <c r="V29" s="182"/>
+      <c r="W29" s="182"/>
+      <c r="X29" s="183"/>
+      <c r="Y29" s="181" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z29" s="182"/>
+      <c r="AA29" s="182"/>
+      <c r="AB29" s="182"/>
+      <c r="AC29" s="182"/>
+      <c r="AD29" s="182"/>
+      <c r="AE29" s="183"/>
+      <c r="AF29" s="137" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG29" s="138"/>
+      <c r="AH29" s="138"/>
+      <c r="AI29" s="138"/>
+      <c r="AJ29" s="138"/>
+      <c r="AK29" s="138"/>
+      <c r="AL29" s="138"/>
+      <c r="AM29" s="139"/>
+      <c r="AN29" s="137" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="121"/>
-      <c r="J29" s="121"/>
-      <c r="K29" s="121"/>
-      <c r="L29" s="121"/>
-      <c r="M29" s="121"/>
-      <c r="N29" s="121"/>
-      <c r="O29" s="121"/>
-      <c r="P29" s="121"/>
-      <c r="Q29" s="121"/>
-      <c r="R29" s="121"/>
-      <c r="S29" s="121"/>
-      <c r="T29" s="121"/>
-      <c r="U29" s="121"/>
-      <c r="V29" s="121"/>
-      <c r="W29" s="121"/>
-      <c r="X29" s="122"/>
-      <c r="Y29" s="120" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z29" s="121"/>
-      <c r="AA29" s="121"/>
-      <c r="AB29" s="121"/>
-      <c r="AC29" s="121"/>
-      <c r="AD29" s="121"/>
-      <c r="AE29" s="122"/>
-      <c r="AF29" s="178" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG29" s="179"/>
-      <c r="AH29" s="179"/>
-      <c r="AI29" s="179"/>
-      <c r="AJ29" s="179"/>
-      <c r="AK29" s="179"/>
-      <c r="AL29" s="179"/>
-      <c r="AM29" s="180"/>
-      <c r="AN29" s="178" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO29" s="179"/>
-      <c r="AP29" s="179"/>
-      <c r="AQ29" s="179"/>
-      <c r="AR29" s="179"/>
-      <c r="AS29" s="179"/>
-      <c r="AT29" s="179"/>
-      <c r="AU29" s="180"/>
+      <c r="AO29" s="138"/>
+      <c r="AP29" s="138"/>
+      <c r="AQ29" s="138"/>
+      <c r="AR29" s="138"/>
+      <c r="AS29" s="138"/>
+      <c r="AT29" s="138"/>
+      <c r="AU29" s="139"/>
       <c r="AV29" s="74"/>
       <c r="AW29" s="51"/>
       <c r="AX29" s="51"/>
     </row>
     <row r="30" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="115"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="123"/>
-      <c r="D30" s="124"/>
-      <c r="E30" s="124"/>
-      <c r="F30" s="124"/>
-      <c r="G30" s="124"/>
-      <c r="H30" s="124"/>
-      <c r="I30" s="124"/>
-      <c r="J30" s="124"/>
-      <c r="K30" s="124"/>
-      <c r="L30" s="124"/>
-      <c r="M30" s="124"/>
-      <c r="N30" s="124"/>
-      <c r="O30" s="124"/>
-      <c r="P30" s="124"/>
-      <c r="Q30" s="124"/>
-      <c r="R30" s="124"/>
-      <c r="S30" s="124"/>
-      <c r="T30" s="124"/>
-      <c r="U30" s="124"/>
-      <c r="V30" s="124"/>
-      <c r="W30" s="124"/>
-      <c r="X30" s="125"/>
-      <c r="Y30" s="123"/>
-      <c r="Z30" s="124"/>
-      <c r="AA30" s="124"/>
-      <c r="AB30" s="124"/>
-      <c r="AC30" s="124"/>
-      <c r="AD30" s="124"/>
-      <c r="AE30" s="125"/>
-      <c r="AF30" s="181"/>
-      <c r="AG30" s="182"/>
-      <c r="AH30" s="182"/>
-      <c r="AI30" s="182"/>
-      <c r="AJ30" s="182"/>
-      <c r="AK30" s="182"/>
-      <c r="AL30" s="182"/>
-      <c r="AM30" s="183"/>
-      <c r="AN30" s="181"/>
-      <c r="AO30" s="182"/>
-      <c r="AP30" s="182"/>
-      <c r="AQ30" s="182"/>
-      <c r="AR30" s="182"/>
-      <c r="AS30" s="182"/>
-      <c r="AT30" s="182"/>
-      <c r="AU30" s="183"/>
+      <c r="A30" s="116"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="184"/>
+      <c r="D30" s="185"/>
+      <c r="E30" s="185"/>
+      <c r="F30" s="185"/>
+      <c r="G30" s="185"/>
+      <c r="H30" s="185"/>
+      <c r="I30" s="185"/>
+      <c r="J30" s="185"/>
+      <c r="K30" s="185"/>
+      <c r="L30" s="185"/>
+      <c r="M30" s="185"/>
+      <c r="N30" s="185"/>
+      <c r="O30" s="185"/>
+      <c r="P30" s="185"/>
+      <c r="Q30" s="185"/>
+      <c r="R30" s="185"/>
+      <c r="S30" s="185"/>
+      <c r="T30" s="185"/>
+      <c r="U30" s="185"/>
+      <c r="V30" s="185"/>
+      <c r="W30" s="185"/>
+      <c r="X30" s="186"/>
+      <c r="Y30" s="184"/>
+      <c r="Z30" s="185"/>
+      <c r="AA30" s="185"/>
+      <c r="AB30" s="185"/>
+      <c r="AC30" s="185"/>
+      <c r="AD30" s="185"/>
+      <c r="AE30" s="186"/>
+      <c r="AF30" s="140"/>
+      <c r="AG30" s="141"/>
+      <c r="AH30" s="141"/>
+      <c r="AI30" s="141"/>
+      <c r="AJ30" s="141"/>
+      <c r="AK30" s="141"/>
+      <c r="AL30" s="141"/>
+      <c r="AM30" s="142"/>
+      <c r="AN30" s="140"/>
+      <c r="AO30" s="141"/>
+      <c r="AP30" s="141"/>
+      <c r="AQ30" s="141"/>
+      <c r="AR30" s="141"/>
+      <c r="AS30" s="141"/>
+      <c r="AT30" s="141"/>
+      <c r="AU30" s="142"/>
       <c r="AV30" s="44"/>
     </row>
     <row r="31" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="126"/>
-      <c r="B31" s="127"/>
+      <c r="A31" s="161"/>
+      <c r="B31" s="163"/>
       <c r="C31" s="83"/>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
@@ -2905,33 +2946,33 @@
       <c r="W31" s="48"/>
       <c r="X31" s="48"/>
       <c r="Y31" s="91"/>
-      <c r="Z31" s="109"/>
-      <c r="AA31" s="109"/>
-      <c r="AB31" s="109"/>
-      <c r="AC31" s="109"/>
-      <c r="AD31" s="109"/>
+      <c r="Z31" s="189"/>
+      <c r="AA31" s="189"/>
+      <c r="AB31" s="189"/>
+      <c r="AC31" s="189"/>
+      <c r="AD31" s="189"/>
       <c r="AE31" s="94"/>
-      <c r="AF31" s="184"/>
-      <c r="AG31" s="185"/>
-      <c r="AH31" s="185"/>
-      <c r="AI31" s="185"/>
-      <c r="AJ31" s="185"/>
-      <c r="AK31" s="185"/>
-      <c r="AL31" s="185"/>
-      <c r="AM31" s="186"/>
+      <c r="AF31" s="143"/>
+      <c r="AG31" s="144"/>
+      <c r="AH31" s="144"/>
+      <c r="AI31" s="144"/>
+      <c r="AJ31" s="144"/>
+      <c r="AK31" s="144"/>
+      <c r="AL31" s="144"/>
+      <c r="AM31" s="145"/>
       <c r="AN31" s="96"/>
-      <c r="AO31" s="190"/>
-      <c r="AP31" s="190"/>
-      <c r="AQ31" s="190"/>
-      <c r="AR31" s="190"/>
-      <c r="AS31" s="190"/>
-      <c r="AT31" s="190"/>
+      <c r="AO31" s="146"/>
+      <c r="AP31" s="146"/>
+      <c r="AQ31" s="146"/>
+      <c r="AR31" s="146"/>
+      <c r="AS31" s="146"/>
+      <c r="AT31" s="146"/>
       <c r="AU31" s="97"/>
       <c r="AV31" s="44"/>
     </row>
     <row r="32" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="111"/>
-      <c r="B32" s="112"/>
+      <c r="A32" s="148"/>
+      <c r="B32" s="150"/>
       <c r="C32" s="44"/>
       <c r="D32" s="47"/>
       <c r="E32" s="47"/>
@@ -2955,34 +2996,34 @@
       <c r="W32" s="47"/>
       <c r="X32" s="47"/>
       <c r="Y32" s="86"/>
-      <c r="Z32" s="110"/>
-      <c r="AA32" s="110"/>
-      <c r="AB32" s="110"/>
-      <c r="AC32" s="110"/>
-      <c r="AD32" s="110"/>
+      <c r="Z32" s="187"/>
+      <c r="AA32" s="187"/>
+      <c r="AB32" s="187"/>
+      <c r="AC32" s="187"/>
+      <c r="AD32" s="187"/>
       <c r="AE32" s="93"/>
-      <c r="AF32" s="117"/>
-      <c r="AG32" s="118"/>
-      <c r="AH32" s="118"/>
-      <c r="AI32" s="118"/>
-      <c r="AJ32" s="118"/>
-      <c r="AK32" s="118"/>
-      <c r="AL32" s="118"/>
-      <c r="AM32" s="119"/>
+      <c r="AF32" s="107"/>
+      <c r="AG32" s="108"/>
+      <c r="AH32" s="108"/>
+      <c r="AI32" s="108"/>
+      <c r="AJ32" s="108"/>
+      <c r="AK32" s="108"/>
+      <c r="AL32" s="108"/>
+      <c r="AM32" s="109"/>
       <c r="AN32" s="74"/>
-      <c r="AO32" s="191"/>
-      <c r="AP32" s="191"/>
-      <c r="AQ32" s="191"/>
-      <c r="AR32" s="191"/>
-      <c r="AS32" s="191"/>
-      <c r="AT32" s="191"/>
+      <c r="AO32" s="106"/>
+      <c r="AP32" s="106"/>
+      <c r="AQ32" s="106"/>
+      <c r="AR32" s="106"/>
+      <c r="AS32" s="106"/>
+      <c r="AT32" s="106"/>
       <c r="AU32" s="98"/>
       <c r="AV32" s="74"/>
       <c r="AX32" s="53"/>
     </row>
     <row r="33" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="111"/>
-      <c r="B33" s="112"/>
+      <c r="A33" s="148"/>
+      <c r="B33" s="150"/>
       <c r="C33" s="44"/>
       <c r="D33" s="47"/>
       <c r="E33" s="47"/>
@@ -3006,34 +3047,34 @@
       <c r="W33" s="47"/>
       <c r="X33" s="47"/>
       <c r="Y33" s="86"/>
-      <c r="Z33" s="110"/>
-      <c r="AA33" s="110"/>
-      <c r="AB33" s="110"/>
-      <c r="AC33" s="110"/>
-      <c r="AD33" s="110"/>
+      <c r="Z33" s="187"/>
+      <c r="AA33" s="187"/>
+      <c r="AB33" s="187"/>
+      <c r="AC33" s="187"/>
+      <c r="AD33" s="187"/>
       <c r="AE33" s="93"/>
-      <c r="AF33" s="117"/>
-      <c r="AG33" s="118"/>
-      <c r="AH33" s="118"/>
-      <c r="AI33" s="118"/>
-      <c r="AJ33" s="118"/>
-      <c r="AK33" s="118"/>
-      <c r="AL33" s="118"/>
-      <c r="AM33" s="119"/>
+      <c r="AF33" s="107"/>
+      <c r="AG33" s="108"/>
+      <c r="AH33" s="108"/>
+      <c r="AI33" s="108"/>
+      <c r="AJ33" s="108"/>
+      <c r="AK33" s="108"/>
+      <c r="AL33" s="108"/>
+      <c r="AM33" s="109"/>
       <c r="AN33" s="74"/>
-      <c r="AO33" s="191"/>
-      <c r="AP33" s="191"/>
-      <c r="AQ33" s="191"/>
-      <c r="AR33" s="191"/>
-      <c r="AS33" s="191"/>
-      <c r="AT33" s="191"/>
+      <c r="AO33" s="106"/>
+      <c r="AP33" s="106"/>
+      <c r="AQ33" s="106"/>
+      <c r="AR33" s="106"/>
+      <c r="AS33" s="106"/>
+      <c r="AT33" s="106"/>
       <c r="AU33" s="98"/>
       <c r="AV33" s="74"/>
       <c r="AX33" s="53"/>
     </row>
     <row r="34" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="111"/>
-      <c r="B34" s="112"/>
+      <c r="A34" s="148"/>
+      <c r="B34" s="150"/>
       <c r="C34" s="44"/>
       <c r="D34" s="47"/>
       <c r="E34" s="47"/>
@@ -3057,33 +3098,33 @@
       <c r="W34" s="47"/>
       <c r="X34" s="47"/>
       <c r="Y34" s="86"/>
-      <c r="Z34" s="110"/>
-      <c r="AA34" s="110"/>
-      <c r="AB34" s="110"/>
-      <c r="AC34" s="110"/>
-      <c r="AD34" s="110"/>
+      <c r="Z34" s="187"/>
+      <c r="AA34" s="187"/>
+      <c r="AB34" s="187"/>
+      <c r="AC34" s="187"/>
+      <c r="AD34" s="187"/>
       <c r="AE34" s="93"/>
-      <c r="AF34" s="117"/>
-      <c r="AG34" s="118"/>
-      <c r="AH34" s="118"/>
-      <c r="AI34" s="118"/>
-      <c r="AJ34" s="118"/>
-      <c r="AK34" s="118"/>
-      <c r="AL34" s="118"/>
-      <c r="AM34" s="119"/>
+      <c r="AF34" s="107"/>
+      <c r="AG34" s="108"/>
+      <c r="AH34" s="108"/>
+      <c r="AI34" s="108"/>
+      <c r="AJ34" s="108"/>
+      <c r="AK34" s="108"/>
+      <c r="AL34" s="108"/>
+      <c r="AM34" s="109"/>
       <c r="AN34" s="74"/>
-      <c r="AO34" s="191"/>
-      <c r="AP34" s="191"/>
-      <c r="AQ34" s="191"/>
-      <c r="AR34" s="191"/>
-      <c r="AS34" s="191"/>
-      <c r="AT34" s="191"/>
+      <c r="AO34" s="106"/>
+      <c r="AP34" s="106"/>
+      <c r="AQ34" s="106"/>
+      <c r="AR34" s="106"/>
+      <c r="AS34" s="106"/>
+      <c r="AT34" s="106"/>
       <c r="AU34" s="98"/>
       <c r="AV34" s="74"/>
     </row>
     <row r="35" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="111"/>
-      <c r="B35" s="112"/>
+      <c r="A35" s="148"/>
+      <c r="B35" s="150"/>
       <c r="C35" s="44"/>
       <c r="D35" s="47"/>
       <c r="E35" s="47"/>
@@ -3107,33 +3148,33 @@
       <c r="W35" s="47"/>
       <c r="X35" s="47"/>
       <c r="Y35" s="86"/>
-      <c r="Z35" s="110"/>
-      <c r="AA35" s="110"/>
-      <c r="AB35" s="110"/>
-      <c r="AC35" s="110"/>
-      <c r="AD35" s="110"/>
+      <c r="Z35" s="187"/>
+      <c r="AA35" s="187"/>
+      <c r="AB35" s="187"/>
+      <c r="AC35" s="187"/>
+      <c r="AD35" s="187"/>
       <c r="AE35" s="93"/>
-      <c r="AF35" s="117"/>
-      <c r="AG35" s="118"/>
-      <c r="AH35" s="118"/>
-      <c r="AI35" s="118"/>
-      <c r="AJ35" s="118"/>
-      <c r="AK35" s="118"/>
-      <c r="AL35" s="118"/>
-      <c r="AM35" s="119"/>
+      <c r="AF35" s="107"/>
+      <c r="AG35" s="108"/>
+      <c r="AH35" s="108"/>
+      <c r="AI35" s="108"/>
+      <c r="AJ35" s="108"/>
+      <c r="AK35" s="108"/>
+      <c r="AL35" s="108"/>
+      <c r="AM35" s="109"/>
       <c r="AN35" s="74"/>
-      <c r="AO35" s="191"/>
-      <c r="AP35" s="191"/>
-      <c r="AQ35" s="191"/>
-      <c r="AR35" s="191"/>
-      <c r="AS35" s="191"/>
-      <c r="AT35" s="191"/>
+      <c r="AO35" s="106"/>
+      <c r="AP35" s="106"/>
+      <c r="AQ35" s="106"/>
+      <c r="AR35" s="106"/>
+      <c r="AS35" s="106"/>
+      <c r="AT35" s="106"/>
       <c r="AU35" s="98"/>
       <c r="AV35" s="44"/>
     </row>
     <row r="36" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="111"/>
-      <c r="B36" s="112"/>
+      <c r="A36" s="148"/>
+      <c r="B36" s="150"/>
       <c r="C36" s="44"/>
       <c r="D36" s="47"/>
       <c r="E36" s="47"/>
@@ -3157,35 +3198,35 @@
       <c r="W36" s="47"/>
       <c r="X36" s="47"/>
       <c r="Y36" s="86"/>
-      <c r="Z36" s="110"/>
-      <c r="AA36" s="110"/>
-      <c r="AB36" s="110"/>
-      <c r="AC36" s="110"/>
-      <c r="AD36" s="110"/>
+      <c r="Z36" s="187"/>
+      <c r="AA36" s="187"/>
+      <c r="AB36" s="187"/>
+      <c r="AC36" s="187"/>
+      <c r="AD36" s="187"/>
       <c r="AE36" s="93"/>
-      <c r="AF36" s="117"/>
-      <c r="AG36" s="118"/>
-      <c r="AH36" s="118"/>
-      <c r="AI36" s="118"/>
-      <c r="AJ36" s="118"/>
-      <c r="AK36" s="118"/>
-      <c r="AL36" s="118"/>
-      <c r="AM36" s="119"/>
+      <c r="AF36" s="107"/>
+      <c r="AG36" s="108"/>
+      <c r="AH36" s="108"/>
+      <c r="AI36" s="108"/>
+      <c r="AJ36" s="108"/>
+      <c r="AK36" s="108"/>
+      <c r="AL36" s="108"/>
+      <c r="AM36" s="109"/>
       <c r="AN36" s="74"/>
-      <c r="AO36" s="191"/>
-      <c r="AP36" s="191"/>
-      <c r="AQ36" s="191"/>
-      <c r="AR36" s="191"/>
-      <c r="AS36" s="191"/>
-      <c r="AT36" s="191"/>
+      <c r="AO36" s="106"/>
+      <c r="AP36" s="106"/>
+      <c r="AQ36" s="106"/>
+      <c r="AR36" s="106"/>
+      <c r="AS36" s="106"/>
+      <c r="AT36" s="106"/>
       <c r="AU36" s="98"/>
       <c r="AV36" s="74"/>
       <c r="AW36" s="51"/>
       <c r="AX36" s="51"/>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A37" s="107"/>
-      <c r="B37" s="108"/>
+      <c r="A37" s="190"/>
+      <c r="B37" s="191"/>
       <c r="C37" s="14"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -3209,33 +3250,33 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
       <c r="Y37" s="92"/>
-      <c r="Z37" s="106"/>
-      <c r="AA37" s="106"/>
-      <c r="AB37" s="106"/>
-      <c r="AC37" s="106"/>
-      <c r="AD37" s="106"/>
+      <c r="Z37" s="188"/>
+      <c r="AA37" s="188"/>
+      <c r="AB37" s="188"/>
+      <c r="AC37" s="188"/>
+      <c r="AD37" s="188"/>
       <c r="AE37" s="95"/>
-      <c r="AF37" s="187"/>
-      <c r="AG37" s="188"/>
-      <c r="AH37" s="188"/>
-      <c r="AI37" s="188"/>
-      <c r="AJ37" s="188"/>
-      <c r="AK37" s="188"/>
-      <c r="AL37" s="188"/>
-      <c r="AM37" s="189"/>
+      <c r="AF37" s="110"/>
+      <c r="AG37" s="111"/>
+      <c r="AH37" s="111"/>
+      <c r="AI37" s="111"/>
+      <c r="AJ37" s="111"/>
+      <c r="AK37" s="111"/>
+      <c r="AL37" s="111"/>
+      <c r="AM37" s="112"/>
       <c r="AN37" s="74"/>
-      <c r="AO37" s="191"/>
-      <c r="AP37" s="191"/>
-      <c r="AQ37" s="191"/>
-      <c r="AR37" s="191"/>
-      <c r="AS37" s="191"/>
-      <c r="AT37" s="191"/>
+      <c r="AO37" s="106"/>
+      <c r="AP37" s="106"/>
+      <c r="AQ37" s="106"/>
+      <c r="AR37" s="106"/>
+      <c r="AS37" s="106"/>
+      <c r="AT37" s="106"/>
       <c r="AU37" s="98"/>
       <c r="AV37" s="14"/>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A38" s="107"/>
-      <c r="B38" s="108"/>
+      <c r="A38" s="190"/>
+      <c r="B38" s="191"/>
       <c r="C38" s="14"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -3259,33 +3300,33 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="92"/>
-      <c r="Z38" s="106"/>
-      <c r="AA38" s="106"/>
-      <c r="AB38" s="106"/>
-      <c r="AC38" s="106"/>
-      <c r="AD38" s="106"/>
+      <c r="Z38" s="188"/>
+      <c r="AA38" s="188"/>
+      <c r="AB38" s="188"/>
+      <c r="AC38" s="188"/>
+      <c r="AD38" s="188"/>
       <c r="AE38" s="95"/>
-      <c r="AF38" s="187"/>
-      <c r="AG38" s="188"/>
-      <c r="AH38" s="188"/>
-      <c r="AI38" s="188"/>
-      <c r="AJ38" s="188"/>
-      <c r="AK38" s="188"/>
-      <c r="AL38" s="188"/>
-      <c r="AM38" s="189"/>
+      <c r="AF38" s="110"/>
+      <c r="AG38" s="111"/>
+      <c r="AH38" s="111"/>
+      <c r="AI38" s="111"/>
+      <c r="AJ38" s="111"/>
+      <c r="AK38" s="111"/>
+      <c r="AL38" s="111"/>
+      <c r="AM38" s="112"/>
       <c r="AN38" s="74"/>
-      <c r="AO38" s="191"/>
-      <c r="AP38" s="191"/>
-      <c r="AQ38" s="191"/>
-      <c r="AR38" s="191"/>
-      <c r="AS38" s="191"/>
-      <c r="AT38" s="191"/>
+      <c r="AO38" s="106"/>
+      <c r="AP38" s="106"/>
+      <c r="AQ38" s="106"/>
+      <c r="AR38" s="106"/>
+      <c r="AS38" s="106"/>
+      <c r="AT38" s="106"/>
       <c r="AU38" s="98"/>
       <c r="AV38" s="14"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A39" s="107"/>
-      <c r="B39" s="108"/>
+      <c r="A39" s="190"/>
+      <c r="B39" s="191"/>
       <c r="C39" s="14"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -3309,33 +3350,33 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
       <c r="Y39" s="92"/>
-      <c r="Z39" s="106"/>
-      <c r="AA39" s="106"/>
-      <c r="AB39" s="106"/>
-      <c r="AC39" s="106"/>
-      <c r="AD39" s="106"/>
+      <c r="Z39" s="188"/>
+      <c r="AA39" s="188"/>
+      <c r="AB39" s="188"/>
+      <c r="AC39" s="188"/>
+      <c r="AD39" s="188"/>
       <c r="AE39" s="95"/>
-      <c r="AF39" s="187"/>
-      <c r="AG39" s="188"/>
-      <c r="AH39" s="188"/>
-      <c r="AI39" s="188"/>
-      <c r="AJ39" s="188"/>
-      <c r="AK39" s="188"/>
-      <c r="AL39" s="188"/>
-      <c r="AM39" s="189"/>
+      <c r="AF39" s="110"/>
+      <c r="AG39" s="111"/>
+      <c r="AH39" s="111"/>
+      <c r="AI39" s="111"/>
+      <c r="AJ39" s="111"/>
+      <c r="AK39" s="111"/>
+      <c r="AL39" s="111"/>
+      <c r="AM39" s="112"/>
       <c r="AN39" s="74"/>
-      <c r="AO39" s="191"/>
-      <c r="AP39" s="191"/>
-      <c r="AQ39" s="191"/>
-      <c r="AR39" s="191"/>
-      <c r="AS39" s="191"/>
-      <c r="AT39" s="191"/>
+      <c r="AO39" s="106"/>
+      <c r="AP39" s="106"/>
+      <c r="AQ39" s="106"/>
+      <c r="AR39" s="106"/>
+      <c r="AS39" s="106"/>
+      <c r="AT39" s="106"/>
       <c r="AU39" s="98"/>
       <c r="AV39" s="14"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A40" s="107"/>
-      <c r="B40" s="108"/>
+      <c r="A40" s="190"/>
+      <c r="B40" s="191"/>
       <c r="C40" s="14"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -3359,27 +3400,27 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
       <c r="Y40" s="92"/>
-      <c r="Z40" s="106"/>
-      <c r="AA40" s="106"/>
-      <c r="AB40" s="106"/>
-      <c r="AC40" s="106"/>
-      <c r="AD40" s="106"/>
+      <c r="Z40" s="188"/>
+      <c r="AA40" s="188"/>
+      <c r="AB40" s="188"/>
+      <c r="AC40" s="188"/>
+      <c r="AD40" s="188"/>
       <c r="AE40" s="95"/>
-      <c r="AF40" s="187"/>
-      <c r="AG40" s="188"/>
-      <c r="AH40" s="188"/>
-      <c r="AI40" s="188"/>
-      <c r="AJ40" s="188"/>
-      <c r="AK40" s="188"/>
-      <c r="AL40" s="188"/>
-      <c r="AM40" s="189"/>
+      <c r="AF40" s="110"/>
+      <c r="AG40" s="111"/>
+      <c r="AH40" s="111"/>
+      <c r="AI40" s="111"/>
+      <c r="AJ40" s="111"/>
+      <c r="AK40" s="111"/>
+      <c r="AL40" s="111"/>
+      <c r="AM40" s="112"/>
       <c r="AN40" s="74"/>
-      <c r="AO40" s="191"/>
-      <c r="AP40" s="191"/>
-      <c r="AQ40" s="191"/>
-      <c r="AR40" s="191"/>
-      <c r="AS40" s="191"/>
-      <c r="AT40" s="191"/>
+      <c r="AO40" s="106"/>
+      <c r="AP40" s="106"/>
+      <c r="AQ40" s="106"/>
+      <c r="AR40" s="106"/>
+      <c r="AS40" s="106"/>
+      <c r="AT40" s="106"/>
       <c r="AU40" s="98"/>
       <c r="AV40" s="14"/>
     </row>
@@ -3484,55 +3525,55 @@
       <c r="AV42" s="14"/>
     </row>
     <row r="43" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="146" t="s">
-        <v>40</v>
+      <c r="A43" s="122" t="s">
+        <v>38</v>
       </c>
-      <c r="B43" s="147"/>
-      <c r="C43" s="147"/>
-      <c r="D43" s="147"/>
-      <c r="E43" s="147"/>
-      <c r="F43" s="147"/>
-      <c r="G43" s="147"/>
-      <c r="H43" s="147"/>
-      <c r="I43" s="147"/>
-      <c r="J43" s="147"/>
-      <c r="K43" s="147"/>
-      <c r="L43" s="147"/>
-      <c r="M43" s="147"/>
-      <c r="N43" s="147"/>
-      <c r="O43" s="147"/>
-      <c r="P43" s="147"/>
-      <c r="Q43" s="147"/>
-      <c r="R43" s="147"/>
-      <c r="S43" s="147"/>
-      <c r="T43" s="147"/>
-      <c r="U43" s="147"/>
-      <c r="V43" s="147"/>
-      <c r="W43" s="147"/>
-      <c r="X43" s="147"/>
-      <c r="Y43" s="147"/>
-      <c r="Z43" s="147"/>
-      <c r="AA43" s="147"/>
-      <c r="AB43" s="147"/>
-      <c r="AC43" s="147"/>
-      <c r="AD43" s="147"/>
-      <c r="AE43" s="147"/>
-      <c r="AF43" s="147"/>
-      <c r="AG43" s="147"/>
-      <c r="AH43" s="147"/>
-      <c r="AI43" s="147"/>
-      <c r="AJ43" s="147"/>
-      <c r="AK43" s="147"/>
-      <c r="AL43" s="147"/>
-      <c r="AM43" s="147"/>
-      <c r="AN43" s="147"/>
-      <c r="AO43" s="147"/>
-      <c r="AP43" s="147"/>
-      <c r="AQ43" s="147"/>
-      <c r="AR43" s="147"/>
-      <c r="AS43" s="147"/>
-      <c r="AT43" s="147"/>
-      <c r="AU43" s="148"/>
+      <c r="B43" s="123"/>
+      <c r="C43" s="123"/>
+      <c r="D43" s="123"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="123"/>
+      <c r="H43" s="123"/>
+      <c r="I43" s="123"/>
+      <c r="J43" s="123"/>
+      <c r="K43" s="123"/>
+      <c r="L43" s="123"/>
+      <c r="M43" s="123"/>
+      <c r="N43" s="123"/>
+      <c r="O43" s="123"/>
+      <c r="P43" s="123"/>
+      <c r="Q43" s="123"/>
+      <c r="R43" s="123"/>
+      <c r="S43" s="123"/>
+      <c r="T43" s="123"/>
+      <c r="U43" s="123"/>
+      <c r="V43" s="123"/>
+      <c r="W43" s="123"/>
+      <c r="X43" s="123"/>
+      <c r="Y43" s="123"/>
+      <c r="Z43" s="123"/>
+      <c r="AA43" s="123"/>
+      <c r="AB43" s="123"/>
+      <c r="AC43" s="123"/>
+      <c r="AD43" s="123"/>
+      <c r="AE43" s="123"/>
+      <c r="AF43" s="123"/>
+      <c r="AG43" s="123"/>
+      <c r="AH43" s="123"/>
+      <c r="AI43" s="123"/>
+      <c r="AJ43" s="123"/>
+      <c r="AK43" s="123"/>
+      <c r="AL43" s="123"/>
+      <c r="AM43" s="123"/>
+      <c r="AN43" s="123"/>
+      <c r="AO43" s="123"/>
+      <c r="AP43" s="123"/>
+      <c r="AQ43" s="123"/>
+      <c r="AR43" s="123"/>
+      <c r="AS43" s="123"/>
+      <c r="AT43" s="123"/>
+      <c r="AU43" s="124"/>
       <c r="AV43" s="14"/>
     </row>
     <row r="44" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3587,7 +3628,7 @@
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A45" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -3612,8 +3653,8 @@
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
-      <c r="Y45" s="128"/>
-      <c r="Z45" s="130"/>
+      <c r="Y45" s="156"/>
+      <c r="Z45" s="158"/>
       <c r="AA45" s="4"/>
       <c r="AB45" s="4"/>
       <c r="AC45" s="4"/>
@@ -3969,7 +4010,7 @@
       <c r="AC52" s="87"/>
       <c r="AD52" s="87"/>
       <c r="AE52" s="90" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AF52" s="90"/>
       <c r="AG52" s="90"/>
@@ -3979,18 +4020,18 @@
       <c r="AK52" s="90"/>
       <c r="AL52" s="90"/>
       <c r="AM52" s="90"/>
-      <c r="AN52" s="163" t="s">
+      <c r="AN52" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="AO52" s="163"/>
-      <c r="AP52" s="164">
+      <c r="AO52" s="113"/>
+      <c r="AP52" s="114">
         <v>0</v>
       </c>
-      <c r="AQ52" s="164"/>
-      <c r="AR52" s="164"/>
-      <c r="AS52" s="164"/>
-      <c r="AT52" s="164"/>
-      <c r="AU52" s="165"/>
+      <c r="AQ52" s="114"/>
+      <c r="AR52" s="114"/>
+      <c r="AS52" s="114"/>
+      <c r="AT52" s="114"/>
+      <c r="AU52" s="115"/>
       <c r="AV52" s="14"/>
     </row>
     <row r="53" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3999,7 +4040,7 @@
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="20"/>
@@ -4149,7 +4190,7 @@
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -4243,10 +4284,10 @@
       <c r="AO57" s="8"/>
       <c r="AP57" s="8"/>
       <c r="AQ57" s="3"/>
-      <c r="AR57" s="131"/>
-      <c r="AS57" s="131"/>
-      <c r="AT57" s="131"/>
-      <c r="AU57" s="132"/>
+      <c r="AR57" s="159"/>
+      <c r="AS57" s="159"/>
+      <c r="AT57" s="159"/>
+      <c r="AU57" s="160"/>
       <c r="AV57" s="14"/>
     </row>
     <row r="58" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4350,55 +4391,55 @@
       <c r="AV59" s="14"/>
     </row>
     <row r="60" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="146" t="s">
-        <v>43</v>
+      <c r="A60" s="122" t="s">
+        <v>41</v>
       </c>
-      <c r="B60" s="147"/>
-      <c r="C60" s="147"/>
-      <c r="D60" s="147"/>
-      <c r="E60" s="147"/>
-      <c r="F60" s="147"/>
-      <c r="G60" s="147"/>
-      <c r="H60" s="147"/>
-      <c r="I60" s="147"/>
-      <c r="J60" s="147"/>
-      <c r="K60" s="147"/>
-      <c r="L60" s="147"/>
-      <c r="M60" s="147"/>
-      <c r="N60" s="147"/>
-      <c r="O60" s="147"/>
-      <c r="P60" s="147"/>
-      <c r="Q60" s="147"/>
-      <c r="R60" s="147"/>
-      <c r="S60" s="147"/>
-      <c r="T60" s="147"/>
-      <c r="U60" s="147"/>
-      <c r="V60" s="147"/>
-      <c r="W60" s="147"/>
-      <c r="X60" s="147"/>
-      <c r="Y60" s="147"/>
-      <c r="Z60" s="147"/>
-      <c r="AA60" s="147"/>
-      <c r="AB60" s="147"/>
-      <c r="AC60" s="147"/>
-      <c r="AD60" s="147"/>
-      <c r="AE60" s="147"/>
-      <c r="AF60" s="147"/>
-      <c r="AG60" s="147"/>
-      <c r="AH60" s="147"/>
-      <c r="AI60" s="147"/>
-      <c r="AJ60" s="147"/>
-      <c r="AK60" s="147"/>
-      <c r="AL60" s="147"/>
-      <c r="AM60" s="147"/>
-      <c r="AN60" s="147"/>
-      <c r="AO60" s="147"/>
-      <c r="AP60" s="147"/>
-      <c r="AQ60" s="147"/>
-      <c r="AR60" s="147"/>
-      <c r="AS60" s="147"/>
-      <c r="AT60" s="147"/>
-      <c r="AU60" s="148"/>
+      <c r="B60" s="123"/>
+      <c r="C60" s="123"/>
+      <c r="D60" s="123"/>
+      <c r="E60" s="123"/>
+      <c r="F60" s="123"/>
+      <c r="G60" s="123"/>
+      <c r="H60" s="123"/>
+      <c r="I60" s="123"/>
+      <c r="J60" s="123"/>
+      <c r="K60" s="123"/>
+      <c r="L60" s="123"/>
+      <c r="M60" s="123"/>
+      <c r="N60" s="123"/>
+      <c r="O60" s="123"/>
+      <c r="P60" s="123"/>
+      <c r="Q60" s="123"/>
+      <c r="R60" s="123"/>
+      <c r="S60" s="123"/>
+      <c r="T60" s="123"/>
+      <c r="U60" s="123"/>
+      <c r="V60" s="123"/>
+      <c r="W60" s="123"/>
+      <c r="X60" s="123"/>
+      <c r="Y60" s="123"/>
+      <c r="Z60" s="123"/>
+      <c r="AA60" s="123"/>
+      <c r="AB60" s="123"/>
+      <c r="AC60" s="123"/>
+      <c r="AD60" s="123"/>
+      <c r="AE60" s="123"/>
+      <c r="AF60" s="123"/>
+      <c r="AG60" s="123"/>
+      <c r="AH60" s="123"/>
+      <c r="AI60" s="123"/>
+      <c r="AJ60" s="123"/>
+      <c r="AK60" s="123"/>
+      <c r="AL60" s="123"/>
+      <c r="AM60" s="123"/>
+      <c r="AN60" s="123"/>
+      <c r="AO60" s="123"/>
+      <c r="AP60" s="123"/>
+      <c r="AQ60" s="123"/>
+      <c r="AR60" s="123"/>
+      <c r="AS60" s="123"/>
+      <c r="AT60" s="123"/>
+      <c r="AU60" s="124"/>
       <c r="AV60" s="14"/>
     </row>
     <row r="61" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4452,57 +4493,57 @@
       <c r="AV61" s="14"/>
     </row>
     <row r="62" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A62" s="126" t="s">
+      <c r="A62" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="162"/>
+      <c r="C62" s="162"/>
+      <c r="D62" s="162"/>
+      <c r="E62" s="162"/>
+      <c r="F62" s="162"/>
+      <c r="G62" s="162"/>
+      <c r="H62" s="162"/>
+      <c r="I62" s="162"/>
+      <c r="J62" s="162"/>
+      <c r="K62" s="162"/>
+      <c r="L62" s="162"/>
+      <c r="M62" s="162"/>
+      <c r="N62" s="162"/>
+      <c r="O62" s="162"/>
+      <c r="P62" s="162"/>
+      <c r="Q62" s="162"/>
+      <c r="R62" s="162"/>
+      <c r="S62" s="162"/>
+      <c r="T62" s="162"/>
+      <c r="U62" s="162"/>
+      <c r="V62" s="162"/>
+      <c r="W62" s="162"/>
+      <c r="X62" s="162"/>
+      <c r="Y62" s="163"/>
+      <c r="Z62" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="133"/>
-      <c r="C62" s="133"/>
-      <c r="D62" s="133"/>
-      <c r="E62" s="133"/>
-      <c r="F62" s="133"/>
-      <c r="G62" s="133"/>
-      <c r="H62" s="133"/>
-      <c r="I62" s="133"/>
-      <c r="J62" s="133"/>
-      <c r="K62" s="133"/>
-      <c r="L62" s="133"/>
-      <c r="M62" s="133"/>
-      <c r="N62" s="133"/>
-      <c r="O62" s="133"/>
-      <c r="P62" s="133"/>
-      <c r="Q62" s="133"/>
-      <c r="R62" s="133"/>
-      <c r="S62" s="133"/>
-      <c r="T62" s="133"/>
-      <c r="U62" s="133"/>
-      <c r="V62" s="133"/>
-      <c r="W62" s="133"/>
-      <c r="X62" s="133"/>
-      <c r="Y62" s="127"/>
-      <c r="Z62" s="126" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA62" s="133"/>
-      <c r="AB62" s="133"/>
-      <c r="AC62" s="133"/>
-      <c r="AD62" s="133"/>
-      <c r="AE62" s="133"/>
-      <c r="AF62" s="133"/>
-      <c r="AG62" s="133"/>
-      <c r="AH62" s="133"/>
-      <c r="AI62" s="133"/>
-      <c r="AJ62" s="133"/>
-      <c r="AK62" s="133"/>
-      <c r="AL62" s="133"/>
-      <c r="AM62" s="133"/>
-      <c r="AN62" s="133"/>
-      <c r="AO62" s="133"/>
-      <c r="AP62" s="133"/>
-      <c r="AQ62" s="133"/>
-      <c r="AR62" s="133"/>
-      <c r="AS62" s="133"/>
-      <c r="AT62" s="133"/>
-      <c r="AU62" s="127"/>
+      <c r="AA62" s="162"/>
+      <c r="AB62" s="162"/>
+      <c r="AC62" s="162"/>
+      <c r="AD62" s="162"/>
+      <c r="AE62" s="162"/>
+      <c r="AF62" s="162"/>
+      <c r="AG62" s="162"/>
+      <c r="AH62" s="162"/>
+      <c r="AI62" s="162"/>
+      <c r="AJ62" s="162"/>
+      <c r="AK62" s="162"/>
+      <c r="AL62" s="162"/>
+      <c r="AM62" s="162"/>
+      <c r="AN62" s="162"/>
+      <c r="AO62" s="162"/>
+      <c r="AP62" s="162"/>
+      <c r="AQ62" s="162"/>
+      <c r="AR62" s="162"/>
+      <c r="AS62" s="162"/>
+      <c r="AT62" s="162"/>
+      <c r="AU62" s="163"/>
       <c r="AV62" s="14"/>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.2">
@@ -4941,16 +4982,16 @@
       <c r="AG71" s="2"/>
       <c r="AH71" s="4"/>
       <c r="AI71" s="4"/>
-      <c r="AJ71" s="130"/>
-      <c r="AK71" s="130"/>
-      <c r="AL71" s="130"/>
-      <c r="AM71" s="130"/>
-      <c r="AN71" s="130"/>
-      <c r="AO71" s="130"/>
-      <c r="AP71" s="130"/>
-      <c r="AQ71" s="130"/>
-      <c r="AR71" s="130"/>
-      <c r="AS71" s="130"/>
+      <c r="AJ71" s="158"/>
+      <c r="AK71" s="158"/>
+      <c r="AL71" s="158"/>
+      <c r="AM71" s="158"/>
+      <c r="AN71" s="158"/>
+      <c r="AO71" s="158"/>
+      <c r="AP71" s="158"/>
+      <c r="AQ71" s="158"/>
+      <c r="AR71" s="158"/>
+      <c r="AS71" s="158"/>
       <c r="AT71" s="4"/>
       <c r="AU71" s="10"/>
       <c r="AV71" s="14"/>
@@ -5011,17 +5052,56 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="AO40:AT40"/>
-    <mergeCell ref="AF36:AM36"/>
-    <mergeCell ref="AF37:AM37"/>
-    <mergeCell ref="AO34:AT34"/>
-    <mergeCell ref="AO35:AT35"/>
-    <mergeCell ref="AO36:AT36"/>
-    <mergeCell ref="AO37:AT37"/>
-    <mergeCell ref="AO38:AT38"/>
-    <mergeCell ref="AO39:AT39"/>
-    <mergeCell ref="AF38:AM38"/>
-    <mergeCell ref="AF39:AM39"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="Z36:AD36"/>
+    <mergeCell ref="Z37:AD37"/>
+    <mergeCell ref="Z40:AD40"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="Z38:AD38"/>
+    <mergeCell ref="Z32:AD32"/>
+    <mergeCell ref="Z33:AD33"/>
+    <mergeCell ref="Z34:AD34"/>
+    <mergeCell ref="Z35:AD35"/>
+    <mergeCell ref="Z39:AD39"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="AF32:AM32"/>
+    <mergeCell ref="AF33:AM33"/>
+    <mergeCell ref="AF34:AM34"/>
+    <mergeCell ref="AF35:AM35"/>
+    <mergeCell ref="Y29:AE30"/>
+    <mergeCell ref="C29:X30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="Z31:AD31"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AM6:AS6"/>
+    <mergeCell ref="AJ71:AS71"/>
+    <mergeCell ref="AR57:AU57"/>
+    <mergeCell ref="Z62:AU62"/>
+    <mergeCell ref="Y45:Z45"/>
+    <mergeCell ref="AJ24:AM25"/>
+    <mergeCell ref="AF24:AI25"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="A62:Y62"/>
+    <mergeCell ref="A10:AU10"/>
+    <mergeCell ref="A17:AU17"/>
+    <mergeCell ref="A60:AU60"/>
+    <mergeCell ref="AN24:AU25"/>
+    <mergeCell ref="AN27:AU27"/>
+    <mergeCell ref="A24:B25"/>
+    <mergeCell ref="Y13:AE13"/>
+    <mergeCell ref="AJ27:AM27"/>
+    <mergeCell ref="AJ28:AM28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="L15:AT15"/>
+    <mergeCell ref="AL13:AT13"/>
     <mergeCell ref="AN52:AO52"/>
     <mergeCell ref="AP52:AU52"/>
     <mergeCell ref="A22:M22"/>
@@ -5038,56 +5118,17 @@
     <mergeCell ref="AO31:AT31"/>
     <mergeCell ref="AO32:AT32"/>
     <mergeCell ref="AO33:AT33"/>
-    <mergeCell ref="A24:B25"/>
-    <mergeCell ref="Y13:AE13"/>
-    <mergeCell ref="AJ27:AM27"/>
-    <mergeCell ref="AJ28:AM28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="L15:AT15"/>
-    <mergeCell ref="AL13:AT13"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AM6:AS6"/>
-    <mergeCell ref="AJ71:AS71"/>
-    <mergeCell ref="AR57:AU57"/>
-    <mergeCell ref="Z62:AU62"/>
-    <mergeCell ref="Y45:Z45"/>
-    <mergeCell ref="AJ24:AM25"/>
-    <mergeCell ref="AF24:AI25"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="AF28:AI28"/>
-    <mergeCell ref="A62:Y62"/>
-    <mergeCell ref="A10:AU10"/>
-    <mergeCell ref="A17:AU17"/>
-    <mergeCell ref="A60:AU60"/>
-    <mergeCell ref="AN24:AU25"/>
-    <mergeCell ref="AN27:AU27"/>
-    <mergeCell ref="A29:B30"/>
-    <mergeCell ref="AF32:AM32"/>
-    <mergeCell ref="AF33:AM33"/>
-    <mergeCell ref="AF34:AM34"/>
-    <mergeCell ref="AF35:AM35"/>
-    <mergeCell ref="Y29:AE30"/>
-    <mergeCell ref="C29:X30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="Z36:AD36"/>
-    <mergeCell ref="Z37:AD37"/>
-    <mergeCell ref="Z40:AD40"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="Z38:AD38"/>
-    <mergeCell ref="Z31:AD31"/>
-    <mergeCell ref="Z32:AD32"/>
-    <mergeCell ref="Z33:AD33"/>
-    <mergeCell ref="Z34:AD34"/>
-    <mergeCell ref="Z35:AD35"/>
-    <mergeCell ref="Z39:AD39"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="AO40:AT40"/>
+    <mergeCell ref="AF36:AM36"/>
+    <mergeCell ref="AF37:AM37"/>
+    <mergeCell ref="AO34:AT34"/>
+    <mergeCell ref="AO35:AT35"/>
+    <mergeCell ref="AO36:AT36"/>
+    <mergeCell ref="AO37:AT37"/>
+    <mergeCell ref="AO38:AT38"/>
+    <mergeCell ref="AO39:AT39"/>
+    <mergeCell ref="AF38:AM38"/>
+    <mergeCell ref="AF39:AM39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.51181102362204722" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificacion en certificado de aceptacion
</commit_message>
<xml_diff>
--- a/public/file_layouts/OC_Certificate_model.xlsx
+++ b/public/file_layouts/OC_Certificate_model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\services\public\file_layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EB7C78CE-7A02-4AF4-8B9E-F134D3FEBFD4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E913821-467E-4C60-9EEB-352417966C26}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="253" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,21 @@
     <sheet name="Certificado" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Certificado!$A$1:$AU$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Certificado!$A$1:$AU$73</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Cant</t>
   </si>
@@ -125,13 +132,7 @@
     <t>FIRMA AUTORIZACIÓN GERENCIA GENERAL</t>
   </si>
   <si>
-    <t>No. de recepción parcial:</t>
-  </si>
-  <si>
     <t>Código:</t>
-  </si>
-  <si>
-    <t>Fecha</t>
   </si>
   <si>
     <t>Monto</t>
@@ -171,6 +172,15 @@
   </si>
   <si>
     <t>Historial</t>
+  </si>
+  <si>
+    <t>CC:</t>
+  </si>
+  <si>
+    <t>No. de certificación:</t>
+  </si>
+  <si>
+    <t>Fecha de emisión</t>
   </si>
 </sst>
 </file>
@@ -427,7 +437,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -641,6 +651,54 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,6 +708,213 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -659,242 +924,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1301,10 +1332,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AX73"/>
+  <dimension ref="A1:AX74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AW14" sqref="AW14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AP31" sqref="AP31:AT41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1437,10 +1468,10 @@
       <c r="AJ2" s="4"/>
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
-      <c r="AM2" s="156"/>
-      <c r="AN2" s="156"/>
-      <c r="AO2" s="156"/>
-      <c r="AP2" s="156"/>
+      <c r="AM2" s="137"/>
+      <c r="AN2" s="137"/>
+      <c r="AO2" s="137"/>
+      <c r="AP2" s="137"/>
       <c r="AQ2" s="22"/>
       <c r="AR2" s="4"/>
       <c r="AS2" s="4"/>
@@ -1643,13 +1674,13 @@
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
       <c r="AL6" s="4"/>
-      <c r="AM6" s="157"/>
-      <c r="AN6" s="157"/>
-      <c r="AO6" s="157"/>
-      <c r="AP6" s="157"/>
-      <c r="AQ6" s="157"/>
-      <c r="AR6" s="157"/>
-      <c r="AS6" s="157"/>
+      <c r="AM6" s="138"/>
+      <c r="AN6" s="138"/>
+      <c r="AO6" s="138"/>
+      <c r="AP6" s="138"/>
+      <c r="AQ6" s="138"/>
+      <c r="AR6" s="138"/>
+      <c r="AS6" s="138"/>
       <c r="AT6" s="22"/>
       <c r="AU6" s="23"/>
       <c r="AV6" s="14"/>
@@ -1687,7 +1718,7 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="77" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AG7" s="4"/>
       <c r="AH7" s="4"/>
@@ -1807,55 +1838,55 @@
       <c r="AV9" s="14"/>
     </row>
     <row r="10" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="123"/>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="123"/>
-      <c r="L10" s="123"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="123"/>
-      <c r="P10" s="123"/>
-      <c r="Q10" s="123"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="123"/>
-      <c r="T10" s="123"/>
-      <c r="U10" s="123"/>
-      <c r="V10" s="123"/>
-      <c r="W10" s="123"/>
-      <c r="X10" s="123"/>
-      <c r="Y10" s="123"/>
-      <c r="Z10" s="123"/>
-      <c r="AA10" s="123"/>
-      <c r="AB10" s="123"/>
-      <c r="AC10" s="123"/>
-      <c r="AD10" s="123"/>
-      <c r="AE10" s="123"/>
-      <c r="AF10" s="123"/>
-      <c r="AG10" s="123"/>
-      <c r="AH10" s="123"/>
-      <c r="AI10" s="123"/>
-      <c r="AJ10" s="123"/>
-      <c r="AK10" s="123"/>
-      <c r="AL10" s="123"/>
-      <c r="AM10" s="123"/>
-      <c r="AN10" s="123"/>
-      <c r="AO10" s="123"/>
-      <c r="AP10" s="123"/>
-      <c r="AQ10" s="123"/>
-      <c r="AR10" s="123"/>
-      <c r="AS10" s="123"/>
-      <c r="AT10" s="123"/>
-      <c r="AU10" s="124"/>
+      <c r="B10" s="156"/>
+      <c r="C10" s="156"/>
+      <c r="D10" s="156"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="156"/>
+      <c r="H10" s="156"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
+      <c r="M10" s="156"/>
+      <c r="N10" s="156"/>
+      <c r="O10" s="156"/>
+      <c r="P10" s="156"/>
+      <c r="Q10" s="156"/>
+      <c r="R10" s="156"/>
+      <c r="S10" s="156"/>
+      <c r="T10" s="156"/>
+      <c r="U10" s="156"/>
+      <c r="V10" s="156"/>
+      <c r="W10" s="156"/>
+      <c r="X10" s="156"/>
+      <c r="Y10" s="156"/>
+      <c r="Z10" s="156"/>
+      <c r="AA10" s="156"/>
+      <c r="AB10" s="156"/>
+      <c r="AC10" s="156"/>
+      <c r="AD10" s="156"/>
+      <c r="AE10" s="156"/>
+      <c r="AF10" s="156"/>
+      <c r="AG10" s="156"/>
+      <c r="AH10" s="156"/>
+      <c r="AI10" s="156"/>
+      <c r="AJ10" s="156"/>
+      <c r="AK10" s="156"/>
+      <c r="AL10" s="156"/>
+      <c r="AM10" s="156"/>
+      <c r="AN10" s="156"/>
+      <c r="AO10" s="156"/>
+      <c r="AP10" s="156"/>
+      <c r="AQ10" s="156"/>
+      <c r="AR10" s="156"/>
+      <c r="AS10" s="156"/>
+      <c r="AT10" s="156"/>
+      <c r="AU10" s="157"/>
       <c r="AV10" s="14"/>
     </row>
     <row r="11" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1942,21 +1973,23 @@
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
+      <c r="AF12" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
       <c r="AJ12" s="6"/>
       <c r="AK12" s="6"/>
-      <c r="AL12" s="6"/>
-      <c r="AM12" s="6"/>
-      <c r="AN12" s="6"/>
-      <c r="AO12" s="6"/>
-      <c r="AP12" s="6"/>
-      <c r="AQ12" s="6"/>
-      <c r="AR12" s="6"/>
-      <c r="AS12" s="8"/>
-      <c r="AT12" s="8"/>
+      <c r="AL12" s="171"/>
+      <c r="AM12" s="171"/>
+      <c r="AN12" s="171"/>
+      <c r="AO12" s="171"/>
+      <c r="AP12" s="171"/>
+      <c r="AQ12" s="171"/>
+      <c r="AR12" s="171"/>
+      <c r="AS12" s="171"/>
+      <c r="AT12" s="171"/>
       <c r="AU12" s="11"/>
       <c r="AV12" s="14"/>
     </row>
@@ -1987,30 +2020,30 @@
       <c r="V13" s="16"/>
       <c r="W13" s="19"/>
       <c r="X13" s="16"/>
-      <c r="Y13" s="147"/>
-      <c r="Z13" s="147"/>
-      <c r="AA13" s="147"/>
-      <c r="AB13" s="147"/>
-      <c r="AC13" s="147"/>
-      <c r="AD13" s="147"/>
-      <c r="AE13" s="147"/>
+      <c r="Y13" s="166"/>
+      <c r="Z13" s="166"/>
+      <c r="AA13" s="166"/>
+      <c r="AB13" s="166"/>
+      <c r="AC13" s="166"/>
+      <c r="AD13" s="166"/>
+      <c r="AE13" s="166"/>
       <c r="AF13" s="46" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AG13" s="20"/>
       <c r="AH13" s="15"/>
       <c r="AI13" s="15"/>
       <c r="AJ13" s="15"/>
       <c r="AK13" s="15"/>
-      <c r="AL13" s="155"/>
-      <c r="AM13" s="155"/>
-      <c r="AN13" s="155"/>
-      <c r="AO13" s="155"/>
-      <c r="AP13" s="155"/>
-      <c r="AQ13" s="155"/>
-      <c r="AR13" s="155"/>
-      <c r="AS13" s="155"/>
-      <c r="AT13" s="155"/>
+      <c r="AL13" s="172"/>
+      <c r="AM13" s="172"/>
+      <c r="AN13" s="172"/>
+      <c r="AO13" s="172"/>
+      <c r="AP13" s="172"/>
+      <c r="AQ13" s="172"/>
+      <c r="AR13" s="172"/>
+      <c r="AS13" s="172"/>
+      <c r="AT13" s="172"/>
       <c r="AU13" s="27"/>
       <c r="AV13" s="14"/>
     </row>
@@ -2049,7 +2082,7 @@
       <c r="AD14" s="15"/>
       <c r="AE14" s="15"/>
       <c r="AF14" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AG14" s="38"/>
       <c r="AH14" s="15"/>
@@ -2082,41 +2115,41 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="154"/>
-      <c r="M15" s="154"/>
-      <c r="N15" s="154"/>
-      <c r="O15" s="154"/>
-      <c r="P15" s="154"/>
-      <c r="Q15" s="154"/>
-      <c r="R15" s="154"/>
-      <c r="S15" s="154"/>
-      <c r="T15" s="154"/>
-      <c r="U15" s="154"/>
-      <c r="V15" s="154"/>
-      <c r="W15" s="154"/>
-      <c r="X15" s="154"/>
-      <c r="Y15" s="154"/>
-      <c r="Z15" s="154"/>
-      <c r="AA15" s="154"/>
-      <c r="AB15" s="154"/>
-      <c r="AC15" s="154"/>
-      <c r="AD15" s="154"/>
-      <c r="AE15" s="154"/>
-      <c r="AF15" s="154"/>
-      <c r="AG15" s="154"/>
-      <c r="AH15" s="154"/>
-      <c r="AI15" s="154"/>
-      <c r="AJ15" s="154"/>
-      <c r="AK15" s="154"/>
-      <c r="AL15" s="154"/>
-      <c r="AM15" s="154"/>
-      <c r="AN15" s="154"/>
-      <c r="AO15" s="154"/>
-      <c r="AP15" s="154"/>
-      <c r="AQ15" s="154"/>
-      <c r="AR15" s="154"/>
-      <c r="AS15" s="154"/>
-      <c r="AT15" s="154"/>
+      <c r="L15" s="171"/>
+      <c r="M15" s="171"/>
+      <c r="N15" s="171"/>
+      <c r="O15" s="171"/>
+      <c r="P15" s="171"/>
+      <c r="Q15" s="171"/>
+      <c r="R15" s="171"/>
+      <c r="S15" s="171"/>
+      <c r="T15" s="171"/>
+      <c r="U15" s="171"/>
+      <c r="V15" s="171"/>
+      <c r="W15" s="171"/>
+      <c r="X15" s="171"/>
+      <c r="Y15" s="171"/>
+      <c r="Z15" s="171"/>
+      <c r="AA15" s="171"/>
+      <c r="AB15" s="171"/>
+      <c r="AC15" s="171"/>
+      <c r="AD15" s="171"/>
+      <c r="AE15" s="171"/>
+      <c r="AF15" s="171"/>
+      <c r="AG15" s="171"/>
+      <c r="AH15" s="171"/>
+      <c r="AI15" s="171"/>
+      <c r="AJ15" s="171"/>
+      <c r="AK15" s="171"/>
+      <c r="AL15" s="171"/>
+      <c r="AM15" s="171"/>
+      <c r="AN15" s="171"/>
+      <c r="AO15" s="171"/>
+      <c r="AP15" s="171"/>
+      <c r="AQ15" s="171"/>
+      <c r="AR15" s="171"/>
+      <c r="AS15" s="171"/>
+      <c r="AT15" s="171"/>
       <c r="AU15" s="10"/>
       <c r="AV15" s="14"/>
     </row>
@@ -2171,55 +2204,55 @@
       <c r="AV16" s="14"/>
     </row>
     <row r="17" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="123"/>
-      <c r="J17" s="123"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="123"/>
-      <c r="P17" s="123"/>
-      <c r="Q17" s="123"/>
-      <c r="R17" s="123"/>
-      <c r="S17" s="123"/>
-      <c r="T17" s="123"/>
-      <c r="U17" s="123"/>
-      <c r="V17" s="123"/>
-      <c r="W17" s="123"/>
-      <c r="X17" s="123"/>
-      <c r="Y17" s="123"/>
-      <c r="Z17" s="123"/>
-      <c r="AA17" s="123"/>
-      <c r="AB17" s="123"/>
-      <c r="AC17" s="123"/>
-      <c r="AD17" s="123"/>
-      <c r="AE17" s="123"/>
-      <c r="AF17" s="123"/>
-      <c r="AG17" s="123"/>
-      <c r="AH17" s="123"/>
-      <c r="AI17" s="123"/>
-      <c r="AJ17" s="123"/>
-      <c r="AK17" s="123"/>
-      <c r="AL17" s="123"/>
-      <c r="AM17" s="123"/>
-      <c r="AN17" s="123"/>
-      <c r="AO17" s="123"/>
-      <c r="AP17" s="123"/>
-      <c r="AQ17" s="123"/>
-      <c r="AR17" s="123"/>
-      <c r="AS17" s="123"/>
-      <c r="AT17" s="123"/>
-      <c r="AU17" s="124"/>
+      <c r="B17" s="156"/>
+      <c r="C17" s="156"/>
+      <c r="D17" s="156"/>
+      <c r="E17" s="156"/>
+      <c r="F17" s="156"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
+      <c r="K17" s="156"/>
+      <c r="L17" s="156"/>
+      <c r="M17" s="156"/>
+      <c r="N17" s="156"/>
+      <c r="O17" s="156"/>
+      <c r="P17" s="156"/>
+      <c r="Q17" s="156"/>
+      <c r="R17" s="156"/>
+      <c r="S17" s="156"/>
+      <c r="T17" s="156"/>
+      <c r="U17" s="156"/>
+      <c r="V17" s="156"/>
+      <c r="W17" s="156"/>
+      <c r="X17" s="156"/>
+      <c r="Y17" s="156"/>
+      <c r="Z17" s="156"/>
+      <c r="AA17" s="156"/>
+      <c r="AB17" s="156"/>
+      <c r="AC17" s="156"/>
+      <c r="AD17" s="156"/>
+      <c r="AE17" s="156"/>
+      <c r="AF17" s="156"/>
+      <c r="AG17" s="156"/>
+      <c r="AH17" s="156"/>
+      <c r="AI17" s="156"/>
+      <c r="AJ17" s="156"/>
+      <c r="AK17" s="156"/>
+      <c r="AL17" s="156"/>
+      <c r="AM17" s="156"/>
+      <c r="AN17" s="156"/>
+      <c r="AO17" s="156"/>
+      <c r="AP17" s="156"/>
+      <c r="AQ17" s="156"/>
+      <c r="AR17" s="156"/>
+      <c r="AS17" s="156"/>
+      <c r="AT17" s="156"/>
+      <c r="AU17" s="157"/>
       <c r="AV17" s="14"/>
     </row>
     <row r="18" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2307,7 +2340,7 @@
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
       <c r="AB19" s="47" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="AC19" s="4"/>
       <c r="AD19" s="4"/>
@@ -2439,39 +2472,39 @@
       <c r="AV21" s="14"/>
     </row>
     <row r="22" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="116"/>
-      <c r="B22" s="117"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="117"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="117"/>
-      <c r="L22" s="117"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="119"/>
-      <c r="O22" s="120"/>
-      <c r="P22" s="120"/>
-      <c r="Q22" s="120"/>
-      <c r="R22" s="120"/>
-      <c r="S22" s="120"/>
-      <c r="T22" s="120"/>
-      <c r="U22" s="120"/>
-      <c r="V22" s="120"/>
-      <c r="W22" s="120"/>
-      <c r="X22" s="120"/>
-      <c r="Y22" s="121"/>
-      <c r="Z22" s="119"/>
-      <c r="AA22" s="120"/>
-      <c r="AB22" s="120"/>
-      <c r="AC22" s="120"/>
-      <c r="AD22" s="120"/>
-      <c r="AE22" s="120"/>
-      <c r="AF22" s="120"/>
-      <c r="AG22" s="121"/>
+      <c r="A22" s="160"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="176"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="176"/>
+      <c r="H22" s="176"/>
+      <c r="I22" s="176"/>
+      <c r="J22" s="176"/>
+      <c r="K22" s="176"/>
+      <c r="L22" s="176"/>
+      <c r="M22" s="161"/>
+      <c r="N22" s="177"/>
+      <c r="O22" s="178"/>
+      <c r="P22" s="178"/>
+      <c r="Q22" s="178"/>
+      <c r="R22" s="178"/>
+      <c r="S22" s="178"/>
+      <c r="T22" s="178"/>
+      <c r="U22" s="178"/>
+      <c r="V22" s="178"/>
+      <c r="W22" s="178"/>
+      <c r="X22" s="178"/>
+      <c r="Y22" s="179"/>
+      <c r="Z22" s="177"/>
+      <c r="AA22" s="178"/>
+      <c r="AB22" s="178"/>
+      <c r="AC22" s="178"/>
+      <c r="AD22" s="178"/>
+      <c r="AE22" s="178"/>
+      <c r="AF22" s="178"/>
+      <c r="AG22" s="179"/>
       <c r="AH22" s="60"/>
       <c r="AI22" s="16"/>
       <c r="AJ22" s="16"/>
@@ -2539,113 +2572,113 @@
       <c r="AV23" s="14"/>
     </row>
     <row r="24" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="125" t="s">
+      <c r="A24" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="127"/>
-      <c r="C24" s="125" t="s">
+      <c r="B24" s="163"/>
+      <c r="C24" s="162" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="126"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="126"/>
-      <c r="I24" s="126"/>
-      <c r="J24" s="126"/>
-      <c r="K24" s="126"/>
-      <c r="L24" s="126"/>
-      <c r="M24" s="126"/>
-      <c r="N24" s="126"/>
-      <c r="O24" s="126"/>
-      <c r="P24" s="126"/>
-      <c r="Q24" s="126"/>
-      <c r="R24" s="126"/>
-      <c r="S24" s="126"/>
-      <c r="T24" s="126"/>
-      <c r="U24" s="126"/>
-      <c r="V24" s="126"/>
-      <c r="W24" s="126"/>
-      <c r="X24" s="126"/>
-      <c r="Y24" s="126"/>
-      <c r="Z24" s="126"/>
-      <c r="AA24" s="126"/>
-      <c r="AB24" s="126"/>
-      <c r="AC24" s="126"/>
-      <c r="AD24" s="126"/>
-      <c r="AE24" s="127"/>
-      <c r="AF24" s="164" t="s">
+      <c r="D24" s="180"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="180"/>
+      <c r="L24" s="180"/>
+      <c r="M24" s="180"/>
+      <c r="N24" s="180"/>
+      <c r="O24" s="180"/>
+      <c r="P24" s="180"/>
+      <c r="Q24" s="180"/>
+      <c r="R24" s="180"/>
+      <c r="S24" s="180"/>
+      <c r="T24" s="180"/>
+      <c r="U24" s="180"/>
+      <c r="V24" s="180"/>
+      <c r="W24" s="180"/>
+      <c r="X24" s="180"/>
+      <c r="Y24" s="180"/>
+      <c r="Z24" s="180"/>
+      <c r="AA24" s="180"/>
+      <c r="AB24" s="180"/>
+      <c r="AC24" s="180"/>
+      <c r="AD24" s="180"/>
+      <c r="AE24" s="163"/>
+      <c r="AF24" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="AG24" s="165"/>
-      <c r="AH24" s="165"/>
-      <c r="AI24" s="166"/>
-      <c r="AJ24" s="164" t="s">
+      <c r="AG24" s="144"/>
+      <c r="AH24" s="144"/>
+      <c r="AI24" s="145"/>
+      <c r="AJ24" s="143" t="s">
         <v>1</v>
       </c>
-      <c r="AK24" s="165"/>
-      <c r="AL24" s="165"/>
-      <c r="AM24" s="166"/>
-      <c r="AN24" s="164" t="s">
-        <v>36</v>
+      <c r="AK24" s="144"/>
+      <c r="AL24" s="144"/>
+      <c r="AM24" s="145"/>
+      <c r="AN24" s="143" t="s">
+        <v>34</v>
       </c>
-      <c r="AO24" s="165"/>
-      <c r="AP24" s="165"/>
-      <c r="AQ24" s="165"/>
-      <c r="AR24" s="165"/>
-      <c r="AS24" s="165"/>
-      <c r="AT24" s="165"/>
-      <c r="AU24" s="166"/>
+      <c r="AO24" s="144"/>
+      <c r="AP24" s="144"/>
+      <c r="AQ24" s="144"/>
+      <c r="AR24" s="144"/>
+      <c r="AS24" s="144"/>
+      <c r="AT24" s="144"/>
+      <c r="AU24" s="145"/>
       <c r="AV24" s="14"/>
     </row>
     <row r="25" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="128"/>
-      <c r="B25" s="130"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="129"/>
-      <c r="F25" s="129"/>
-      <c r="G25" s="129"/>
-      <c r="H25" s="129"/>
-      <c r="I25" s="129"/>
-      <c r="J25" s="129"/>
-      <c r="K25" s="129"/>
-      <c r="L25" s="129"/>
-      <c r="M25" s="129"/>
-      <c r="N25" s="129"/>
-      <c r="O25" s="129"/>
-      <c r="P25" s="129"/>
-      <c r="Q25" s="129"/>
-      <c r="R25" s="129"/>
-      <c r="S25" s="129"/>
-      <c r="T25" s="129"/>
-      <c r="U25" s="129"/>
-      <c r="V25" s="129"/>
-      <c r="W25" s="129"/>
-      <c r="X25" s="129"/>
-      <c r="Y25" s="129"/>
-      <c r="Z25" s="129"/>
-      <c r="AA25" s="129"/>
-      <c r="AB25" s="129"/>
-      <c r="AC25" s="129"/>
-      <c r="AD25" s="129"/>
-      <c r="AE25" s="130"/>
-      <c r="AF25" s="167"/>
-      <c r="AG25" s="168"/>
-      <c r="AH25" s="168"/>
-      <c r="AI25" s="169"/>
-      <c r="AJ25" s="167"/>
-      <c r="AK25" s="168"/>
-      <c r="AL25" s="168"/>
-      <c r="AM25" s="169"/>
-      <c r="AN25" s="167"/>
-      <c r="AO25" s="168"/>
-      <c r="AP25" s="168"/>
-      <c r="AQ25" s="168"/>
-      <c r="AR25" s="168"/>
-      <c r="AS25" s="168"/>
-      <c r="AT25" s="168"/>
-      <c r="AU25" s="169"/>
+      <c r="A25" s="164"/>
+      <c r="B25" s="165"/>
+      <c r="C25" s="164"/>
+      <c r="D25" s="181"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="181"/>
+      <c r="G25" s="181"/>
+      <c r="H25" s="181"/>
+      <c r="I25" s="181"/>
+      <c r="J25" s="181"/>
+      <c r="K25" s="181"/>
+      <c r="L25" s="181"/>
+      <c r="M25" s="181"/>
+      <c r="N25" s="181"/>
+      <c r="O25" s="181"/>
+      <c r="P25" s="181"/>
+      <c r="Q25" s="181"/>
+      <c r="R25" s="181"/>
+      <c r="S25" s="181"/>
+      <c r="T25" s="181"/>
+      <c r="U25" s="181"/>
+      <c r="V25" s="181"/>
+      <c r="W25" s="181"/>
+      <c r="X25" s="181"/>
+      <c r="Y25" s="181"/>
+      <c r="Z25" s="181"/>
+      <c r="AA25" s="181"/>
+      <c r="AB25" s="181"/>
+      <c r="AC25" s="181"/>
+      <c r="AD25" s="181"/>
+      <c r="AE25" s="165"/>
+      <c r="AF25" s="146"/>
+      <c r="AG25" s="147"/>
+      <c r="AH25" s="147"/>
+      <c r="AI25" s="148"/>
+      <c r="AJ25" s="146"/>
+      <c r="AK25" s="147"/>
+      <c r="AL25" s="147"/>
+      <c r="AM25" s="148"/>
+      <c r="AN25" s="146"/>
+      <c r="AO25" s="147"/>
+      <c r="AP25" s="147"/>
+      <c r="AQ25" s="147"/>
+      <c r="AR25" s="147"/>
+      <c r="AS25" s="147"/>
+      <c r="AT25" s="147"/>
+      <c r="AU25" s="148"/>
       <c r="AV25" s="14"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.2">
@@ -2688,21 +2721,21 @@
       <c r="AK26" s="7"/>
       <c r="AL26" s="7"/>
       <c r="AM26" s="9"/>
-      <c r="AN26" s="131"/>
-      <c r="AO26" s="132"/>
-      <c r="AP26" s="132"/>
-      <c r="AQ26" s="132"/>
-      <c r="AR26" s="132"/>
-      <c r="AS26" s="132"/>
-      <c r="AT26" s="132"/>
-      <c r="AU26" s="133"/>
+      <c r="AN26" s="182"/>
+      <c r="AO26" s="183"/>
+      <c r="AP26" s="183"/>
+      <c r="AQ26" s="183"/>
+      <c r="AR26" s="183"/>
+      <c r="AS26" s="183"/>
+      <c r="AT26" s="183"/>
+      <c r="AU26" s="184"/>
       <c r="AV26" s="14"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A27" s="148">
+      <c r="A27" s="123">
         <v>1</v>
       </c>
-      <c r="B27" s="150"/>
+      <c r="B27" s="124"/>
       <c r="C27" s="44"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
@@ -2732,28 +2765,28 @@
       <c r="AC27" s="47"/>
       <c r="AD27" s="47"/>
       <c r="AE27" s="50"/>
-      <c r="AF27" s="170">
+      <c r="AF27" s="149">
         <v>1</v>
       </c>
-      <c r="AG27" s="171"/>
-      <c r="AH27" s="171"/>
-      <c r="AI27" s="172"/>
-      <c r="AJ27" s="148" t="s">
-        <v>42</v>
+      <c r="AG27" s="150"/>
+      <c r="AH27" s="150"/>
+      <c r="AI27" s="151"/>
+      <c r="AJ27" s="123" t="s">
+        <v>40</v>
       </c>
-      <c r="AK27" s="149"/>
-      <c r="AL27" s="149"/>
-      <c r="AM27" s="150"/>
-      <c r="AN27" s="176">
+      <c r="AK27" s="167"/>
+      <c r="AL27" s="167"/>
+      <c r="AM27" s="124"/>
+      <c r="AN27" s="113"/>
+      <c r="AO27" s="200">
         <v>0</v>
       </c>
-      <c r="AO27" s="177"/>
-      <c r="AP27" s="177"/>
-      <c r="AQ27" s="177"/>
-      <c r="AR27" s="177"/>
-      <c r="AS27" s="177"/>
-      <c r="AT27" s="177"/>
-      <c r="AU27" s="178"/>
+      <c r="AP27" s="200"/>
+      <c r="AQ27" s="200"/>
+      <c r="AR27" s="200"/>
+      <c r="AS27" s="200"/>
+      <c r="AT27" s="200"/>
+      <c r="AU27" s="114"/>
       <c r="AV27" s="14"/>
     </row>
     <row r="28" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
@@ -2788,141 +2821,141 @@
       <c r="AC28" s="49"/>
       <c r="AD28" s="49"/>
       <c r="AE28" s="85"/>
-      <c r="AF28" s="173"/>
-      <c r="AG28" s="174"/>
-      <c r="AH28" s="174"/>
-      <c r="AI28" s="175"/>
-      <c r="AJ28" s="151"/>
-      <c r="AK28" s="152"/>
-      <c r="AL28" s="152"/>
-      <c r="AM28" s="153"/>
-      <c r="AN28" s="134"/>
-      <c r="AO28" s="135"/>
-      <c r="AP28" s="135"/>
-      <c r="AQ28" s="135"/>
-      <c r="AR28" s="135"/>
-      <c r="AS28" s="135"/>
-      <c r="AT28" s="135"/>
-      <c r="AU28" s="136"/>
+      <c r="AF28" s="152"/>
+      <c r="AG28" s="153"/>
+      <c r="AH28" s="153"/>
+      <c r="AI28" s="154"/>
+      <c r="AJ28" s="168"/>
+      <c r="AK28" s="169"/>
+      <c r="AL28" s="169"/>
+      <c r="AM28" s="170"/>
+      <c r="AN28" s="185"/>
+      <c r="AO28" s="186"/>
+      <c r="AP28" s="186"/>
+      <c r="AQ28" s="186"/>
+      <c r="AR28" s="186"/>
+      <c r="AS28" s="186"/>
+      <c r="AT28" s="186"/>
+      <c r="AU28" s="187"/>
       <c r="AV28" s="74"/>
       <c r="AW28" s="51"/>
       <c r="AX28" s="51"/>
     </row>
     <row r="29" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="179" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="180"/>
-      <c r="C29" s="181" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="182"/>
-      <c r="E29" s="182"/>
-      <c r="F29" s="182"/>
-      <c r="G29" s="182"/>
-      <c r="H29" s="182"/>
-      <c r="I29" s="182"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="182"/>
-      <c r="L29" s="182"/>
-      <c r="M29" s="182"/>
-      <c r="N29" s="182"/>
-      <c r="O29" s="182"/>
-      <c r="P29" s="182"/>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="182"/>
-      <c r="S29" s="182"/>
-      <c r="T29" s="182"/>
-      <c r="U29" s="182"/>
-      <c r="V29" s="182"/>
-      <c r="W29" s="182"/>
-      <c r="X29" s="183"/>
-      <c r="Y29" s="181" t="s">
+      <c r="A29" s="158" t="s">
         <v>35</v>
       </c>
-      <c r="Z29" s="182"/>
-      <c r="AA29" s="182"/>
-      <c r="AB29" s="182"/>
-      <c r="AC29" s="182"/>
-      <c r="AD29" s="182"/>
-      <c r="AE29" s="183"/>
-      <c r="AF29" s="137" t="s">
-        <v>30</v>
+      <c r="B29" s="159"/>
+      <c r="C29" s="128" t="s">
+        <v>41</v>
       </c>
-      <c r="AG29" s="138"/>
-      <c r="AH29" s="138"/>
-      <c r="AI29" s="138"/>
-      <c r="AJ29" s="138"/>
-      <c r="AK29" s="138"/>
-      <c r="AL29" s="138"/>
-      <c r="AM29" s="139"/>
-      <c r="AN29" s="137" t="s">
-        <v>31</v>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="129"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
+      <c r="J29" s="129"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="129"/>
+      <c r="M29" s="129"/>
+      <c r="N29" s="129"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="129"/>
+      <c r="S29" s="129"/>
+      <c r="T29" s="129"/>
+      <c r="U29" s="129"/>
+      <c r="V29" s="129"/>
+      <c r="W29" s="129"/>
+      <c r="X29" s="130"/>
+      <c r="Y29" s="128" t="s">
+        <v>33</v>
       </c>
-      <c r="AO29" s="138"/>
-      <c r="AP29" s="138"/>
-      <c r="AQ29" s="138"/>
-      <c r="AR29" s="138"/>
-      <c r="AS29" s="138"/>
-      <c r="AT29" s="138"/>
-      <c r="AU29" s="139"/>
+      <c r="Z29" s="129"/>
+      <c r="AA29" s="129"/>
+      <c r="AB29" s="129"/>
+      <c r="AC29" s="129"/>
+      <c r="AD29" s="129"/>
+      <c r="AE29" s="130"/>
+      <c r="AF29" s="188" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG29" s="189"/>
+      <c r="AH29" s="189"/>
+      <c r="AI29" s="189"/>
+      <c r="AJ29" s="189"/>
+      <c r="AK29" s="189"/>
+      <c r="AL29" s="189"/>
+      <c r="AM29" s="190"/>
+      <c r="AN29" s="188" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO29" s="189"/>
+      <c r="AP29" s="189"/>
+      <c r="AQ29" s="189"/>
+      <c r="AR29" s="189"/>
+      <c r="AS29" s="189"/>
+      <c r="AT29" s="189"/>
+      <c r="AU29" s="190"/>
       <c r="AV29" s="74"/>
       <c r="AW29" s="51"/>
       <c r="AX29" s="51"/>
     </row>
     <row r="30" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="116"/>
-      <c r="B30" s="118"/>
-      <c r="C30" s="184"/>
-      <c r="D30" s="185"/>
-      <c r="E30" s="185"/>
-      <c r="F30" s="185"/>
-      <c r="G30" s="185"/>
-      <c r="H30" s="185"/>
-      <c r="I30" s="185"/>
-      <c r="J30" s="185"/>
-      <c r="K30" s="185"/>
-      <c r="L30" s="185"/>
-      <c r="M30" s="185"/>
-      <c r="N30" s="185"/>
-      <c r="O30" s="185"/>
-      <c r="P30" s="185"/>
-      <c r="Q30" s="185"/>
-      <c r="R30" s="185"/>
-      <c r="S30" s="185"/>
-      <c r="T30" s="185"/>
-      <c r="U30" s="185"/>
-      <c r="V30" s="185"/>
-      <c r="W30" s="185"/>
-      <c r="X30" s="186"/>
-      <c r="Y30" s="184"/>
-      <c r="Z30" s="185"/>
-      <c r="AA30" s="185"/>
-      <c r="AB30" s="185"/>
-      <c r="AC30" s="185"/>
-      <c r="AD30" s="185"/>
-      <c r="AE30" s="186"/>
-      <c r="AF30" s="140"/>
-      <c r="AG30" s="141"/>
-      <c r="AH30" s="141"/>
-      <c r="AI30" s="141"/>
-      <c r="AJ30" s="141"/>
-      <c r="AK30" s="141"/>
-      <c r="AL30" s="141"/>
-      <c r="AM30" s="142"/>
-      <c r="AN30" s="140"/>
-      <c r="AO30" s="141"/>
-      <c r="AP30" s="141"/>
-      <c r="AQ30" s="141"/>
-      <c r="AR30" s="141"/>
-      <c r="AS30" s="141"/>
-      <c r="AT30" s="141"/>
-      <c r="AU30" s="142"/>
+      <c r="A30" s="160"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="131"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132"/>
+      <c r="H30" s="132"/>
+      <c r="I30" s="132"/>
+      <c r="J30" s="132"/>
+      <c r="K30" s="132"/>
+      <c r="L30" s="132"/>
+      <c r="M30" s="132"/>
+      <c r="N30" s="132"/>
+      <c r="O30" s="132"/>
+      <c r="P30" s="132"/>
+      <c r="Q30" s="132"/>
+      <c r="R30" s="132"/>
+      <c r="S30" s="132"/>
+      <c r="T30" s="132"/>
+      <c r="U30" s="132"/>
+      <c r="V30" s="132"/>
+      <c r="W30" s="132"/>
+      <c r="X30" s="133"/>
+      <c r="Y30" s="131"/>
+      <c r="Z30" s="132"/>
+      <c r="AA30" s="132"/>
+      <c r="AB30" s="132"/>
+      <c r="AC30" s="132"/>
+      <c r="AD30" s="132"/>
+      <c r="AE30" s="133"/>
+      <c r="AF30" s="191"/>
+      <c r="AG30" s="192"/>
+      <c r="AH30" s="192"/>
+      <c r="AI30" s="192"/>
+      <c r="AJ30" s="192"/>
+      <c r="AK30" s="192"/>
+      <c r="AL30" s="192"/>
+      <c r="AM30" s="193"/>
+      <c r="AN30" s="191"/>
+      <c r="AO30" s="192"/>
+      <c r="AP30" s="192"/>
+      <c r="AQ30" s="192"/>
+      <c r="AR30" s="192"/>
+      <c r="AS30" s="192"/>
+      <c r="AT30" s="192"/>
+      <c r="AU30" s="193"/>
       <c r="AV30" s="44"/>
     </row>
     <row r="31" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="161"/>
-      <c r="B31" s="163"/>
+      <c r="A31" s="134"/>
+      <c r="B31" s="135"/>
       <c r="C31" s="83"/>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
@@ -2946,33 +2979,33 @@
       <c r="W31" s="48"/>
       <c r="X31" s="48"/>
       <c r="Y31" s="91"/>
-      <c r="Z31" s="189"/>
-      <c r="AA31" s="189"/>
-      <c r="AB31" s="189"/>
-      <c r="AC31" s="189"/>
-      <c r="AD31" s="189"/>
+      <c r="Z31" s="136"/>
+      <c r="AA31" s="136"/>
+      <c r="AB31" s="136"/>
+      <c r="AC31" s="136"/>
+      <c r="AD31" s="136"/>
       <c r="AE31" s="94"/>
-      <c r="AF31" s="143"/>
-      <c r="AG31" s="144"/>
-      <c r="AH31" s="144"/>
-      <c r="AI31" s="144"/>
-      <c r="AJ31" s="144"/>
-      <c r="AK31" s="144"/>
-      <c r="AL31" s="144"/>
-      <c r="AM31" s="145"/>
+      <c r="AF31" s="194"/>
+      <c r="AG31" s="195"/>
+      <c r="AH31" s="195"/>
+      <c r="AI31" s="195"/>
+      <c r="AJ31" s="195"/>
+      <c r="AK31" s="195"/>
+      <c r="AL31" s="195"/>
+      <c r="AM31" s="196"/>
       <c r="AN31" s="96"/>
-      <c r="AO31" s="146"/>
-      <c r="AP31" s="146"/>
-      <c r="AQ31" s="146"/>
-      <c r="AR31" s="146"/>
-      <c r="AS31" s="146"/>
-      <c r="AT31" s="146"/>
+      <c r="AO31" s="115"/>
+      <c r="AP31" s="116"/>
+      <c r="AQ31" s="116"/>
+      <c r="AR31" s="116"/>
+      <c r="AS31" s="116"/>
+      <c r="AT31" s="116"/>
       <c r="AU31" s="97"/>
       <c r="AV31" s="44"/>
     </row>
     <row r="32" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="148"/>
-      <c r="B32" s="150"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="124"/>
       <c r="C32" s="44"/>
       <c r="D32" s="47"/>
       <c r="E32" s="47"/>
@@ -2996,34 +3029,34 @@
       <c r="W32" s="47"/>
       <c r="X32" s="47"/>
       <c r="Y32" s="86"/>
-      <c r="Z32" s="187"/>
-      <c r="AA32" s="187"/>
-      <c r="AB32" s="187"/>
-      <c r="AC32" s="187"/>
-      <c r="AD32" s="187"/>
+      <c r="Z32" s="121"/>
+      <c r="AA32" s="121"/>
+      <c r="AB32" s="121"/>
+      <c r="AC32" s="121"/>
+      <c r="AD32" s="121"/>
       <c r="AE32" s="93"/>
-      <c r="AF32" s="107"/>
-      <c r="AG32" s="108"/>
-      <c r="AH32" s="108"/>
-      <c r="AI32" s="108"/>
-      <c r="AJ32" s="108"/>
-      <c r="AK32" s="108"/>
-      <c r="AL32" s="108"/>
-      <c r="AM32" s="109"/>
+      <c r="AF32" s="125"/>
+      <c r="AG32" s="126"/>
+      <c r="AH32" s="126"/>
+      <c r="AI32" s="126"/>
+      <c r="AJ32" s="126"/>
+      <c r="AK32" s="126"/>
+      <c r="AL32" s="126"/>
+      <c r="AM32" s="127"/>
       <c r="AN32" s="74"/>
-      <c r="AO32" s="106"/>
-      <c r="AP32" s="106"/>
-      <c r="AQ32" s="106"/>
-      <c r="AR32" s="106"/>
-      <c r="AS32" s="106"/>
-      <c r="AT32" s="106"/>
+      <c r="AO32" s="51"/>
+      <c r="AP32" s="117"/>
+      <c r="AQ32" s="117"/>
+      <c r="AR32" s="117"/>
+      <c r="AS32" s="117"/>
+      <c r="AT32" s="117"/>
       <c r="AU32" s="98"/>
       <c r="AV32" s="74"/>
       <c r="AX32" s="53"/>
     </row>
     <row r="33" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="148"/>
-      <c r="B33" s="150"/>
+      <c r="A33" s="123"/>
+      <c r="B33" s="124"/>
       <c r="C33" s="44"/>
       <c r="D33" s="47"/>
       <c r="E33" s="47"/>
@@ -3047,34 +3080,34 @@
       <c r="W33" s="47"/>
       <c r="X33" s="47"/>
       <c r="Y33" s="86"/>
-      <c r="Z33" s="187"/>
-      <c r="AA33" s="187"/>
-      <c r="AB33" s="187"/>
-      <c r="AC33" s="187"/>
-      <c r="AD33" s="187"/>
+      <c r="Z33" s="121"/>
+      <c r="AA33" s="121"/>
+      <c r="AB33" s="121"/>
+      <c r="AC33" s="121"/>
+      <c r="AD33" s="121"/>
       <c r="AE33" s="93"/>
-      <c r="AF33" s="107"/>
-      <c r="AG33" s="108"/>
-      <c r="AH33" s="108"/>
-      <c r="AI33" s="108"/>
-      <c r="AJ33" s="108"/>
-      <c r="AK33" s="108"/>
-      <c r="AL33" s="108"/>
-      <c r="AM33" s="109"/>
+      <c r="AF33" s="125"/>
+      <c r="AG33" s="126"/>
+      <c r="AH33" s="126"/>
+      <c r="AI33" s="126"/>
+      <c r="AJ33" s="126"/>
+      <c r="AK33" s="126"/>
+      <c r="AL33" s="126"/>
+      <c r="AM33" s="127"/>
       <c r="AN33" s="74"/>
-      <c r="AO33" s="106"/>
-      <c r="AP33" s="106"/>
-      <c r="AQ33" s="106"/>
-      <c r="AR33" s="106"/>
-      <c r="AS33" s="106"/>
-      <c r="AT33" s="106"/>
+      <c r="AO33" s="51"/>
+      <c r="AP33" s="117"/>
+      <c r="AQ33" s="117"/>
+      <c r="AR33" s="117"/>
+      <c r="AS33" s="117"/>
+      <c r="AT33" s="117"/>
       <c r="AU33" s="98"/>
       <c r="AV33" s="74"/>
       <c r="AX33" s="53"/>
     </row>
     <row r="34" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="148"/>
-      <c r="B34" s="150"/>
+      <c r="A34" s="123"/>
+      <c r="B34" s="124"/>
       <c r="C34" s="44"/>
       <c r="D34" s="47"/>
       <c r="E34" s="47"/>
@@ -3098,33 +3131,33 @@
       <c r="W34" s="47"/>
       <c r="X34" s="47"/>
       <c r="Y34" s="86"/>
-      <c r="Z34" s="187"/>
-      <c r="AA34" s="187"/>
-      <c r="AB34" s="187"/>
-      <c r="AC34" s="187"/>
-      <c r="AD34" s="187"/>
+      <c r="Z34" s="121"/>
+      <c r="AA34" s="121"/>
+      <c r="AB34" s="121"/>
+      <c r="AC34" s="121"/>
+      <c r="AD34" s="121"/>
       <c r="AE34" s="93"/>
-      <c r="AF34" s="107"/>
-      <c r="AG34" s="108"/>
-      <c r="AH34" s="108"/>
-      <c r="AI34" s="108"/>
-      <c r="AJ34" s="108"/>
-      <c r="AK34" s="108"/>
-      <c r="AL34" s="108"/>
-      <c r="AM34" s="109"/>
+      <c r="AF34" s="125"/>
+      <c r="AG34" s="126"/>
+      <c r="AH34" s="126"/>
+      <c r="AI34" s="126"/>
+      <c r="AJ34" s="126"/>
+      <c r="AK34" s="126"/>
+      <c r="AL34" s="126"/>
+      <c r="AM34" s="127"/>
       <c r="AN34" s="74"/>
-      <c r="AO34" s="106"/>
-      <c r="AP34" s="106"/>
-      <c r="AQ34" s="106"/>
-      <c r="AR34" s="106"/>
-      <c r="AS34" s="106"/>
-      <c r="AT34" s="106"/>
+      <c r="AO34" s="51"/>
+      <c r="AP34" s="117"/>
+      <c r="AQ34" s="117"/>
+      <c r="AR34" s="117"/>
+      <c r="AS34" s="117"/>
+      <c r="AT34" s="117"/>
       <c r="AU34" s="98"/>
       <c r="AV34" s="74"/>
     </row>
     <row r="35" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="148"/>
-      <c r="B35" s="150"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="124"/>
       <c r="C35" s="44"/>
       <c r="D35" s="47"/>
       <c r="E35" s="47"/>
@@ -3148,33 +3181,33 @@
       <c r="W35" s="47"/>
       <c r="X35" s="47"/>
       <c r="Y35" s="86"/>
-      <c r="Z35" s="187"/>
-      <c r="AA35" s="187"/>
-      <c r="AB35" s="187"/>
-      <c r="AC35" s="187"/>
-      <c r="AD35" s="187"/>
+      <c r="Z35" s="121"/>
+      <c r="AA35" s="121"/>
+      <c r="AB35" s="121"/>
+      <c r="AC35" s="121"/>
+      <c r="AD35" s="121"/>
       <c r="AE35" s="93"/>
-      <c r="AF35" s="107"/>
-      <c r="AG35" s="108"/>
-      <c r="AH35" s="108"/>
-      <c r="AI35" s="108"/>
-      <c r="AJ35" s="108"/>
-      <c r="AK35" s="108"/>
-      <c r="AL35" s="108"/>
-      <c r="AM35" s="109"/>
+      <c r="AF35" s="125"/>
+      <c r="AG35" s="126"/>
+      <c r="AH35" s="126"/>
+      <c r="AI35" s="126"/>
+      <c r="AJ35" s="126"/>
+      <c r="AK35" s="126"/>
+      <c r="AL35" s="126"/>
+      <c r="AM35" s="127"/>
       <c r="AN35" s="74"/>
-      <c r="AO35" s="106"/>
-      <c r="AP35" s="106"/>
-      <c r="AQ35" s="106"/>
-      <c r="AR35" s="106"/>
-      <c r="AS35" s="106"/>
-      <c r="AT35" s="106"/>
+      <c r="AO35" s="51"/>
+      <c r="AP35" s="117"/>
+      <c r="AQ35" s="117"/>
+      <c r="AR35" s="117"/>
+      <c r="AS35" s="117"/>
+      <c r="AT35" s="117"/>
       <c r="AU35" s="98"/>
       <c r="AV35" s="44"/>
     </row>
     <row r="36" spans="1:50" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="148"/>
-      <c r="B36" s="150"/>
+      <c r="A36" s="123"/>
+      <c r="B36" s="124"/>
       <c r="C36" s="44"/>
       <c r="D36" s="47"/>
       <c r="E36" s="47"/>
@@ -3198,35 +3231,35 @@
       <c r="W36" s="47"/>
       <c r="X36" s="47"/>
       <c r="Y36" s="86"/>
-      <c r="Z36" s="187"/>
-      <c r="AA36" s="187"/>
-      <c r="AB36" s="187"/>
-      <c r="AC36" s="187"/>
-      <c r="AD36" s="187"/>
+      <c r="Z36" s="121"/>
+      <c r="AA36" s="121"/>
+      <c r="AB36" s="121"/>
+      <c r="AC36" s="121"/>
+      <c r="AD36" s="121"/>
       <c r="AE36" s="93"/>
-      <c r="AF36" s="107"/>
-      <c r="AG36" s="108"/>
-      <c r="AH36" s="108"/>
-      <c r="AI36" s="108"/>
-      <c r="AJ36" s="108"/>
-      <c r="AK36" s="108"/>
-      <c r="AL36" s="108"/>
-      <c r="AM36" s="109"/>
+      <c r="AF36" s="125"/>
+      <c r="AG36" s="126"/>
+      <c r="AH36" s="126"/>
+      <c r="AI36" s="126"/>
+      <c r="AJ36" s="126"/>
+      <c r="AK36" s="126"/>
+      <c r="AL36" s="126"/>
+      <c r="AM36" s="127"/>
       <c r="AN36" s="74"/>
-      <c r="AO36" s="106"/>
-      <c r="AP36" s="106"/>
-      <c r="AQ36" s="106"/>
-      <c r="AR36" s="106"/>
-      <c r="AS36" s="106"/>
-      <c r="AT36" s="106"/>
+      <c r="AO36" s="51"/>
+      <c r="AP36" s="117"/>
+      <c r="AQ36" s="117"/>
+      <c r="AR36" s="117"/>
+      <c r="AS36" s="117"/>
+      <c r="AT36" s="117"/>
       <c r="AU36" s="98"/>
       <c r="AV36" s="74"/>
       <c r="AW36" s="51"/>
       <c r="AX36" s="51"/>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A37" s="190"/>
-      <c r="B37" s="191"/>
+      <c r="A37" s="119"/>
+      <c r="B37" s="120"/>
       <c r="C37" s="14"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -3250,33 +3283,33 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4"/>
       <c r="Y37" s="92"/>
-      <c r="Z37" s="188"/>
-      <c r="AA37" s="188"/>
-      <c r="AB37" s="188"/>
-      <c r="AC37" s="188"/>
-      <c r="AD37" s="188"/>
+      <c r="Z37" s="122"/>
+      <c r="AA37" s="122"/>
+      <c r="AB37" s="122"/>
+      <c r="AC37" s="122"/>
+      <c r="AD37" s="122"/>
       <c r="AE37" s="95"/>
-      <c r="AF37" s="110"/>
-      <c r="AG37" s="111"/>
-      <c r="AH37" s="111"/>
-      <c r="AI37" s="111"/>
-      <c r="AJ37" s="111"/>
-      <c r="AK37" s="111"/>
-      <c r="AL37" s="111"/>
-      <c r="AM37" s="112"/>
+      <c r="AF37" s="197"/>
+      <c r="AG37" s="198"/>
+      <c r="AH37" s="198"/>
+      <c r="AI37" s="198"/>
+      <c r="AJ37" s="198"/>
+      <c r="AK37" s="198"/>
+      <c r="AL37" s="198"/>
+      <c r="AM37" s="199"/>
       <c r="AN37" s="74"/>
-      <c r="AO37" s="106"/>
-      <c r="AP37" s="106"/>
-      <c r="AQ37" s="106"/>
-      <c r="AR37" s="106"/>
-      <c r="AS37" s="106"/>
-      <c r="AT37" s="106"/>
+      <c r="AO37" s="51"/>
+      <c r="AP37" s="117"/>
+      <c r="AQ37" s="117"/>
+      <c r="AR37" s="117"/>
+      <c r="AS37" s="117"/>
+      <c r="AT37" s="117"/>
       <c r="AU37" s="98"/>
       <c r="AV37" s="14"/>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A38" s="190"/>
-      <c r="B38" s="191"/>
+      <c r="A38" s="119"/>
+      <c r="B38" s="120"/>
       <c r="C38" s="14"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -3300,33 +3333,33 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="92"/>
-      <c r="Z38" s="188"/>
-      <c r="AA38" s="188"/>
-      <c r="AB38" s="188"/>
-      <c r="AC38" s="188"/>
-      <c r="AD38" s="188"/>
+      <c r="Z38" s="122"/>
+      <c r="AA38" s="122"/>
+      <c r="AB38" s="122"/>
+      <c r="AC38" s="122"/>
+      <c r="AD38" s="122"/>
       <c r="AE38" s="95"/>
-      <c r="AF38" s="110"/>
-      <c r="AG38" s="111"/>
-      <c r="AH38" s="111"/>
-      <c r="AI38" s="111"/>
-      <c r="AJ38" s="111"/>
-      <c r="AK38" s="111"/>
-      <c r="AL38" s="111"/>
-      <c r="AM38" s="112"/>
+      <c r="AF38" s="197"/>
+      <c r="AG38" s="198"/>
+      <c r="AH38" s="198"/>
+      <c r="AI38" s="198"/>
+      <c r="AJ38" s="198"/>
+      <c r="AK38" s="198"/>
+      <c r="AL38" s="198"/>
+      <c r="AM38" s="199"/>
       <c r="AN38" s="74"/>
-      <c r="AO38" s="106"/>
-      <c r="AP38" s="106"/>
-      <c r="AQ38" s="106"/>
-      <c r="AR38" s="106"/>
-      <c r="AS38" s="106"/>
-      <c r="AT38" s="106"/>
+      <c r="AO38" s="51"/>
+      <c r="AP38" s="117"/>
+      <c r="AQ38" s="117"/>
+      <c r="AR38" s="117"/>
+      <c r="AS38" s="117"/>
+      <c r="AT38" s="117"/>
       <c r="AU38" s="98"/>
       <c r="AV38" s="14"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A39" s="190"/>
-      <c r="B39" s="191"/>
+      <c r="A39" s="119"/>
+      <c r="B39" s="120"/>
       <c r="C39" s="14"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -3350,33 +3383,33 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4"/>
       <c r="Y39" s="92"/>
-      <c r="Z39" s="188"/>
-      <c r="AA39" s="188"/>
-      <c r="AB39" s="188"/>
-      <c r="AC39" s="188"/>
-      <c r="AD39" s="188"/>
+      <c r="Z39" s="122"/>
+      <c r="AA39" s="122"/>
+      <c r="AB39" s="122"/>
+      <c r="AC39" s="122"/>
+      <c r="AD39" s="122"/>
       <c r="AE39" s="95"/>
-      <c r="AF39" s="110"/>
-      <c r="AG39" s="111"/>
-      <c r="AH39" s="111"/>
-      <c r="AI39" s="111"/>
-      <c r="AJ39" s="111"/>
-      <c r="AK39" s="111"/>
-      <c r="AL39" s="111"/>
-      <c r="AM39" s="112"/>
+      <c r="AF39" s="197"/>
+      <c r="AG39" s="198"/>
+      <c r="AH39" s="198"/>
+      <c r="AI39" s="198"/>
+      <c r="AJ39" s="198"/>
+      <c r="AK39" s="198"/>
+      <c r="AL39" s="198"/>
+      <c r="AM39" s="199"/>
       <c r="AN39" s="74"/>
-      <c r="AO39" s="106"/>
-      <c r="AP39" s="106"/>
-      <c r="AQ39" s="106"/>
-      <c r="AR39" s="106"/>
-      <c r="AS39" s="106"/>
-      <c r="AT39" s="106"/>
+      <c r="AO39" s="51"/>
+      <c r="AP39" s="117"/>
+      <c r="AQ39" s="117"/>
+      <c r="AR39" s="117"/>
+      <c r="AS39" s="117"/>
+      <c r="AT39" s="117"/>
       <c r="AU39" s="98"/>
       <c r="AV39" s="14"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A40" s="190"/>
-      <c r="B40" s="191"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="14"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -3400,236 +3433,234 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4"/>
       <c r="Y40" s="92"/>
-      <c r="Z40" s="188"/>
-      <c r="AA40" s="188"/>
-      <c r="AB40" s="188"/>
-      <c r="AC40" s="188"/>
-      <c r="AD40" s="188"/>
+      <c r="Z40" s="110"/>
+      <c r="AA40" s="110"/>
+      <c r="AB40" s="110"/>
+      <c r="AC40" s="110"/>
+      <c r="AD40" s="110"/>
       <c r="AE40" s="95"/>
-      <c r="AF40" s="110"/>
-      <c r="AG40" s="111"/>
-      <c r="AH40" s="111"/>
-      <c r="AI40" s="111"/>
-      <c r="AJ40" s="111"/>
-      <c r="AK40" s="111"/>
-      <c r="AL40" s="111"/>
-      <c r="AM40" s="112"/>
+      <c r="AF40" s="107"/>
+      <c r="AG40" s="108"/>
+      <c r="AH40" s="108"/>
+      <c r="AI40" s="108"/>
+      <c r="AJ40" s="108"/>
+      <c r="AK40" s="108"/>
+      <c r="AL40" s="108"/>
+      <c r="AM40" s="109"/>
       <c r="AN40" s="74"/>
       <c r="AO40" s="106"/>
-      <c r="AP40" s="106"/>
-      <c r="AQ40" s="106"/>
-      <c r="AR40" s="106"/>
-      <c r="AS40" s="106"/>
-      <c r="AT40" s="106"/>
+      <c r="AP40" s="117"/>
+      <c r="AQ40" s="117"/>
+      <c r="AR40" s="117"/>
+      <c r="AS40" s="117"/>
+      <c r="AT40" s="117"/>
       <c r="AU40" s="98"/>
       <c r="AV40" s="14"/>
     </row>
-    <row r="41" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="104"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="105"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
-      <c r="T41" s="6"/>
-      <c r="U41" s="6"/>
-      <c r="V41" s="6"/>
-      <c r="W41" s="6"/>
-      <c r="X41" s="6"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-      <c r="AA41" s="6"/>
-      <c r="AB41" s="6"/>
-      <c r="AC41" s="6"/>
-      <c r="AD41" s="6"/>
-      <c r="AE41" s="6"/>
-      <c r="AF41" s="6"/>
-      <c r="AG41" s="6"/>
-      <c r="AH41" s="6"/>
-      <c r="AI41" s="6"/>
-      <c r="AJ41" s="6"/>
-      <c r="AK41" s="6"/>
-      <c r="AL41" s="6"/>
-      <c r="AM41" s="6"/>
-      <c r="AN41" s="6"/>
-      <c r="AO41" s="6"/>
-      <c r="AP41" s="6"/>
-      <c r="AQ41" s="6"/>
-      <c r="AR41" s="6"/>
-      <c r="AS41" s="6"/>
-      <c r="AT41" s="6"/>
-      <c r="AU41" s="33"/>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A41" s="119"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="92"/>
+      <c r="Z41" s="122"/>
+      <c r="AA41" s="122"/>
+      <c r="AB41" s="122"/>
+      <c r="AC41" s="122"/>
+      <c r="AD41" s="122"/>
+      <c r="AE41" s="95"/>
+      <c r="AF41" s="197"/>
+      <c r="AG41" s="198"/>
+      <c r="AH41" s="198"/>
+      <c r="AI41" s="198"/>
+      <c r="AJ41" s="198"/>
+      <c r="AK41" s="198"/>
+      <c r="AL41" s="198"/>
+      <c r="AM41" s="199"/>
+      <c r="AN41" s="74"/>
+      <c r="AO41" s="51"/>
+      <c r="AP41" s="118"/>
+      <c r="AQ41" s="118"/>
+      <c r="AR41" s="118"/>
+      <c r="AS41" s="118"/>
+      <c r="AT41" s="118"/>
+      <c r="AU41" s="98"/>
       <c r="AV41" s="14"/>
     </row>
     <row r="42" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="7"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="7"/>
-      <c r="Y42" s="7"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="7"/>
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
-      <c r="AE42" s="7"/>
-      <c r="AF42" s="7"/>
-      <c r="AG42" s="7"/>
-      <c r="AH42" s="7"/>
-      <c r="AI42" s="7"/>
-      <c r="AJ42" s="7"/>
-      <c r="AK42" s="7"/>
-      <c r="AL42" s="7"/>
-      <c r="AM42" s="7"/>
-      <c r="AN42" s="7"/>
-      <c r="AO42" s="7"/>
-      <c r="AP42" s="7"/>
-      <c r="AQ42" s="7"/>
-      <c r="AR42" s="7"/>
-      <c r="AS42" s="7"/>
-      <c r="AT42" s="7"/>
-      <c r="AU42" s="9"/>
+      <c r="A42" s="104"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="105"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
+      <c r="U42" s="6"/>
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+      <c r="X42" s="6"/>
+      <c r="Y42" s="6"/>
+      <c r="Z42" s="6"/>
+      <c r="AA42" s="6"/>
+      <c r="AB42" s="6"/>
+      <c r="AC42" s="6"/>
+      <c r="AD42" s="6"/>
+      <c r="AE42" s="6"/>
+      <c r="AF42" s="6"/>
+      <c r="AG42" s="6"/>
+      <c r="AH42" s="6"/>
+      <c r="AI42" s="6"/>
+      <c r="AJ42" s="6"/>
+      <c r="AK42" s="6"/>
+      <c r="AL42" s="6"/>
+      <c r="AM42" s="6"/>
+      <c r="AN42" s="6"/>
+      <c r="AO42" s="6"/>
+      <c r="AP42" s="6"/>
+      <c r="AQ42" s="6"/>
+      <c r="AR42" s="6"/>
+      <c r="AS42" s="6"/>
+      <c r="AT42" s="6"/>
+      <c r="AU42" s="33"/>
       <c r="AV42" s="14"/>
     </row>
-    <row r="43" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="122" t="s">
-        <v>38</v>
+    <row r="43" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="30"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="7"/>
+      <c r="X43" s="7"/>
+      <c r="Y43" s="7"/>
+      <c r="Z43" s="7"/>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7"/>
+      <c r="AC43" s="7"/>
+      <c r="AD43" s="7"/>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7"/>
+      <c r="AL43" s="7"/>
+      <c r="AM43" s="7"/>
+      <c r="AN43" s="7"/>
+      <c r="AO43" s="7"/>
+      <c r="AP43" s="7"/>
+      <c r="AQ43" s="7"/>
+      <c r="AR43" s="7"/>
+      <c r="AS43" s="7"/>
+      <c r="AT43" s="7"/>
+      <c r="AU43" s="9"/>
+      <c r="AV43" s="14"/>
+    </row>
+    <row r="44" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="155" t="s">
+        <v>36</v>
       </c>
-      <c r="B43" s="123"/>
-      <c r="C43" s="123"/>
-      <c r="D43" s="123"/>
-      <c r="E43" s="123"/>
-      <c r="F43" s="123"/>
-      <c r="G43" s="123"/>
-      <c r="H43" s="123"/>
-      <c r="I43" s="123"/>
-      <c r="J43" s="123"/>
-      <c r="K43" s="123"/>
-      <c r="L43" s="123"/>
-      <c r="M43" s="123"/>
-      <c r="N43" s="123"/>
-      <c r="O43" s="123"/>
-      <c r="P43" s="123"/>
-      <c r="Q43" s="123"/>
-      <c r="R43" s="123"/>
-      <c r="S43" s="123"/>
-      <c r="T43" s="123"/>
-      <c r="U43" s="123"/>
-      <c r="V43" s="123"/>
-      <c r="W43" s="123"/>
-      <c r="X43" s="123"/>
-      <c r="Y43" s="123"/>
-      <c r="Z43" s="123"/>
-      <c r="AA43" s="123"/>
-      <c r="AB43" s="123"/>
-      <c r="AC43" s="123"/>
-      <c r="AD43" s="123"/>
-      <c r="AE43" s="123"/>
-      <c r="AF43" s="123"/>
-      <c r="AG43" s="123"/>
-      <c r="AH43" s="123"/>
-      <c r="AI43" s="123"/>
-      <c r="AJ43" s="123"/>
-      <c r="AK43" s="123"/>
-      <c r="AL43" s="123"/>
-      <c r="AM43" s="123"/>
-      <c r="AN43" s="123"/>
-      <c r="AO43" s="123"/>
-      <c r="AP43" s="123"/>
-      <c r="AQ43" s="123"/>
-      <c r="AR43" s="123"/>
-      <c r="AS43" s="123"/>
-      <c r="AT43" s="123"/>
-      <c r="AU43" s="124"/>
-      <c r="AV43" s="14"/>
-    </row>
-    <row r="44" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="4"/>
-      <c r="Y44" s="4"/>
-      <c r="Z44" s="4"/>
-      <c r="AA44" s="4"/>
-      <c r="AB44" s="4"/>
-      <c r="AC44" s="4"/>
-      <c r="AD44" s="4"/>
-      <c r="AE44" s="4"/>
-      <c r="AF44" s="4"/>
-      <c r="AG44" s="4"/>
-      <c r="AH44" s="4"/>
-      <c r="AI44" s="4"/>
-      <c r="AJ44" s="4"/>
-      <c r="AK44" s="4"/>
-      <c r="AL44" s="4"/>
-      <c r="AM44" s="4"/>
-      <c r="AN44" s="4"/>
-      <c r="AO44" s="4"/>
-      <c r="AP44" s="4"/>
-      <c r="AQ44" s="4"/>
-      <c r="AR44" s="4"/>
-      <c r="AS44" s="4"/>
-      <c r="AT44" s="4"/>
-      <c r="AU44" s="10"/>
+      <c r="B44" s="156"/>
+      <c r="C44" s="156"/>
+      <c r="D44" s="156"/>
+      <c r="E44" s="156"/>
+      <c r="F44" s="156"/>
+      <c r="G44" s="156"/>
+      <c r="H44" s="156"/>
+      <c r="I44" s="156"/>
+      <c r="J44" s="156"/>
+      <c r="K44" s="156"/>
+      <c r="L44" s="156"/>
+      <c r="M44" s="156"/>
+      <c r="N44" s="156"/>
+      <c r="O44" s="156"/>
+      <c r="P44" s="156"/>
+      <c r="Q44" s="156"/>
+      <c r="R44" s="156"/>
+      <c r="S44" s="156"/>
+      <c r="T44" s="156"/>
+      <c r="U44" s="156"/>
+      <c r="V44" s="156"/>
+      <c r="W44" s="156"/>
+      <c r="X44" s="156"/>
+      <c r="Y44" s="156"/>
+      <c r="Z44" s="156"/>
+      <c r="AA44" s="156"/>
+      <c r="AB44" s="156"/>
+      <c r="AC44" s="156"/>
+      <c r="AD44" s="156"/>
+      <c r="AE44" s="156"/>
+      <c r="AF44" s="156"/>
+      <c r="AG44" s="156"/>
+      <c r="AH44" s="156"/>
+      <c r="AI44" s="156"/>
+      <c r="AJ44" s="156"/>
+      <c r="AK44" s="156"/>
+      <c r="AL44" s="156"/>
+      <c r="AM44" s="156"/>
+      <c r="AN44" s="156"/>
+      <c r="AO44" s="156"/>
+      <c r="AP44" s="156"/>
+      <c r="AQ44" s="156"/>
+      <c r="AR44" s="156"/>
+      <c r="AS44" s="156"/>
+      <c r="AT44" s="156"/>
+      <c r="AU44" s="157"/>
       <c r="AV44" s="14"/>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
-        <v>40</v>
-      </c>
+    <row r="45" spans="1:50" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="34"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -3653,8 +3684,8 @@
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
       <c r="X45" s="4"/>
-      <c r="Y45" s="156"/>
-      <c r="Z45" s="158"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
       <c r="AA45" s="4"/>
       <c r="AB45" s="4"/>
       <c r="AC45" s="4"/>
@@ -3679,7 +3710,9 @@
       <c r="AV45" s="14"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
+      <c r="A46" s="31" t="s">
+        <v>38</v>
+      </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -3703,8 +3736,8 @@
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
       <c r="X46" s="4"/>
-      <c r="Y46" s="4"/>
-      <c r="Z46" s="4"/>
+      <c r="Y46" s="137"/>
+      <c r="Z46" s="139"/>
       <c r="AA46" s="4"/>
       <c r="AB46" s="4"/>
       <c r="AC46" s="4"/>
@@ -3929,671 +3962,671 @@
       <c r="AV50" s="14"/>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="8"/>
-      <c r="Y51" s="8"/>
-      <c r="Z51" s="8"/>
-      <c r="AA51" s="8"/>
-      <c r="AB51" s="8"/>
-      <c r="AC51" s="8"/>
-      <c r="AD51" s="8"/>
-      <c r="AE51" s="8"/>
-      <c r="AF51" s="8"/>
-      <c r="AG51" s="8"/>
-      <c r="AH51" s="8"/>
-      <c r="AI51" s="8"/>
-      <c r="AJ51" s="8"/>
-      <c r="AK51" s="8"/>
-      <c r="AL51" s="8"/>
-      <c r="AM51" s="8"/>
-      <c r="AN51" s="8"/>
-      <c r="AO51" s="8"/>
-      <c r="AP51" s="8"/>
-      <c r="AQ51" s="8"/>
-      <c r="AR51" s="8"/>
-      <c r="AS51" s="8"/>
-      <c r="AT51" s="8"/>
-      <c r="AU51" s="11"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="4"/>
+      <c r="AE51" s="4"/>
+      <c r="AF51" s="4"/>
+      <c r="AG51" s="4"/>
+      <c r="AH51" s="4"/>
+      <c r="AI51" s="4"/>
+      <c r="AJ51" s="4"/>
+      <c r="AK51" s="4"/>
+      <c r="AL51" s="4"/>
+      <c r="AM51" s="4"/>
+      <c r="AN51" s="4"/>
+      <c r="AO51" s="4"/>
+      <c r="AP51" s="4"/>
+      <c r="AQ51" s="4"/>
+      <c r="AR51" s="4"/>
+      <c r="AS51" s="4"/>
+      <c r="AT51" s="4"/>
+      <c r="AU51" s="10"/>
       <c r="AV51" s="14"/>
     </row>
-    <row r="52" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="88"/>
-      <c r="B52" s="87"/>
-      <c r="C52" s="87"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="87"/>
-      <c r="I52" s="87"/>
-      <c r="J52" s="87"/>
-      <c r="K52" s="87"/>
-      <c r="L52" s="87"/>
-      <c r="M52" s="87"/>
-      <c r="N52" s="87"/>
-      <c r="O52" s="87"/>
-      <c r="P52" s="87"/>
-      <c r="Q52" s="87"/>
-      <c r="R52" s="87"/>
-      <c r="S52" s="87"/>
-      <c r="T52" s="87"/>
-      <c r="U52" s="89"/>
-      <c r="V52" s="87"/>
-      <c r="W52" s="87"/>
-      <c r="X52" s="87"/>
-      <c r="Y52" s="87"/>
-      <c r="Z52" s="87"/>
-      <c r="AA52" s="87"/>
-      <c r="AB52" s="87"/>
-      <c r="AC52" s="87"/>
-      <c r="AD52" s="87"/>
-      <c r="AE52" s="90" t="s">
-        <v>34</v>
+    <row r="52" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A52" s="13"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="8"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8"/>
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="8"/>
+      <c r="AG52" s="8"/>
+      <c r="AH52" s="8"/>
+      <c r="AI52" s="8"/>
+      <c r="AJ52" s="8"/>
+      <c r="AK52" s="8"/>
+      <c r="AL52" s="8"/>
+      <c r="AM52" s="8"/>
+      <c r="AN52" s="8"/>
+      <c r="AO52" s="8"/>
+      <c r="AP52" s="8"/>
+      <c r="AQ52" s="8"/>
+      <c r="AR52" s="8"/>
+      <c r="AS52" s="8"/>
+      <c r="AT52" s="8"/>
+      <c r="AU52" s="11"/>
+      <c r="AV52" s="14"/>
+    </row>
+    <row r="53" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="88"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
+      <c r="H53" s="87"/>
+      <c r="I53" s="87"/>
+      <c r="J53" s="87"/>
+      <c r="K53" s="87"/>
+      <c r="L53" s="87"/>
+      <c r="M53" s="87"/>
+      <c r="N53" s="87"/>
+      <c r="O53" s="87"/>
+      <c r="P53" s="87"/>
+      <c r="Q53" s="87"/>
+      <c r="R53" s="87"/>
+      <c r="S53" s="87"/>
+      <c r="T53" s="87"/>
+      <c r="U53" s="89"/>
+      <c r="V53" s="87"/>
+      <c r="W53" s="87"/>
+      <c r="X53" s="87"/>
+      <c r="Y53" s="87"/>
+      <c r="Z53" s="87"/>
+      <c r="AA53" s="87"/>
+      <c r="AB53" s="87"/>
+      <c r="AC53" s="87"/>
+      <c r="AD53" s="87"/>
+      <c r="AE53" s="90" t="s">
+        <v>32</v>
       </c>
-      <c r="AF52" s="90"/>
-      <c r="AG52" s="90"/>
-      <c r="AH52" s="90"/>
-      <c r="AI52" s="90"/>
-      <c r="AJ52" s="90"/>
-      <c r="AK52" s="90"/>
-      <c r="AL52" s="90"/>
-      <c r="AM52" s="90"/>
-      <c r="AN52" s="113" t="s">
+      <c r="AF53" s="90"/>
+      <c r="AG53" s="90"/>
+      <c r="AH53" s="90"/>
+      <c r="AI53" s="90"/>
+      <c r="AJ53" s="90"/>
+      <c r="AK53" s="90"/>
+      <c r="AL53" s="90"/>
+      <c r="AM53" s="90"/>
+      <c r="AN53" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="AO52" s="113"/>
-      <c r="AP52" s="114">
+      <c r="AO53" s="173"/>
+      <c r="AP53" s="174">
         <v>0</v>
       </c>
-      <c r="AQ52" s="114"/>
-      <c r="AR52" s="114"/>
-      <c r="AS52" s="114"/>
-      <c r="AT52" s="114"/>
-      <c r="AU52" s="115"/>
-      <c r="AV52" s="14"/>
-    </row>
-    <row r="53" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="26" t="s">
+      <c r="AQ53" s="174"/>
+      <c r="AR53" s="174"/>
+      <c r="AS53" s="174"/>
+      <c r="AT53" s="174"/>
+      <c r="AU53" s="175"/>
+      <c r="AV53" s="14"/>
+    </row>
+    <row r="54" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20" t="s">
+      <c r="B54" s="20"/>
+      <c r="C54" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="20"/>
-      <c r="O53" s="20"/>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="20"/>
-      <c r="R53" s="20"/>
-      <c r="S53" s="20"/>
-      <c r="T53" s="20"/>
-      <c r="U53" s="99"/>
-      <c r="V53" s="20"/>
-      <c r="W53" s="20"/>
-      <c r="X53" s="20"/>
-      <c r="Y53" s="20"/>
-      <c r="Z53" s="20"/>
-      <c r="AA53" s="20"/>
-      <c r="AB53" s="20"/>
-      <c r="AC53" s="20"/>
-      <c r="AD53" s="20"/>
-      <c r="AE53" s="20"/>
-      <c r="AF53" s="20"/>
-      <c r="AG53" s="20"/>
-      <c r="AH53" s="20"/>
-      <c r="AI53" s="20"/>
-      <c r="AJ53" s="20"/>
-      <c r="AK53" s="20"/>
-      <c r="AL53" s="100"/>
-      <c r="AM53" s="100"/>
-      <c r="AN53" s="101"/>
-      <c r="AO53" s="101"/>
-      <c r="AP53" s="102"/>
-      <c r="AQ53" s="102"/>
-      <c r="AR53" s="102"/>
-      <c r="AS53" s="102"/>
-      <c r="AT53" s="102"/>
-      <c r="AU53" s="103"/>
-      <c r="AV53" s="14"/>
-    </row>
-    <row r="54" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="79"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="80"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="6"/>
-      <c r="T54" s="6"/>
-      <c r="U54" s="81"/>
-      <c r="V54" s="6"/>
-      <c r="W54" s="6"/>
-      <c r="X54" s="6"/>
-      <c r="Y54" s="6"/>
-      <c r="Z54" s="6"/>
-      <c r="AA54" s="6"/>
-      <c r="AB54" s="6"/>
-      <c r="AC54" s="6"/>
-      <c r="AD54" s="6"/>
-      <c r="AE54" s="82"/>
-      <c r="AF54" s="6"/>
-      <c r="AG54" s="6"/>
-      <c r="AH54" s="6"/>
-      <c r="AI54" s="6"/>
-      <c r="AJ54" s="6"/>
-      <c r="AK54" s="6"/>
-      <c r="AL54" s="6"/>
-      <c r="AM54" s="6"/>
-      <c r="AN54" s="6"/>
-      <c r="AO54" s="6"/>
-      <c r="AP54" s="6"/>
-      <c r="AQ54" s="6"/>
-      <c r="AR54" s="6"/>
-      <c r="AS54" s="6"/>
-      <c r="AT54" s="6"/>
-      <c r="AU54" s="33"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="20"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="20"/>
+      <c r="T54" s="20"/>
+      <c r="U54" s="99"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="20"/>
+      <c r="X54" s="20"/>
+      <c r="Y54" s="20"/>
+      <c r="Z54" s="20"/>
+      <c r="AA54" s="20"/>
+      <c r="AB54" s="20"/>
+      <c r="AC54" s="20"/>
+      <c r="AD54" s="20"/>
+      <c r="AE54" s="20"/>
+      <c r="AF54" s="20"/>
+      <c r="AG54" s="20"/>
+      <c r="AH54" s="20"/>
+      <c r="AI54" s="20"/>
+      <c r="AJ54" s="20"/>
+      <c r="AK54" s="20"/>
+      <c r="AL54" s="100"/>
+      <c r="AM54" s="100"/>
+      <c r="AN54" s="101"/>
+      <c r="AO54" s="101"/>
+      <c r="AP54" s="102"/>
+      <c r="AQ54" s="102"/>
+      <c r="AR54" s="102"/>
+      <c r="AS54" s="102"/>
+      <c r="AT54" s="102"/>
+      <c r="AU54" s="103"/>
       <c r="AV54" s="14"/>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A55" s="30"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-      <c r="U55" s="7"/>
-      <c r="V55" s="7"/>
-      <c r="W55" s="7"/>
-      <c r="X55" s="7"/>
-      <c r="Y55" s="7"/>
-      <c r="Z55" s="7"/>
-      <c r="AA55" s="7"/>
-      <c r="AB55" s="7"/>
-      <c r="AC55" s="7"/>
-      <c r="AD55" s="7"/>
-      <c r="AE55" s="7"/>
-      <c r="AF55" s="7"/>
-      <c r="AG55" s="7"/>
-      <c r="AH55" s="7"/>
-      <c r="AI55" s="7"/>
-      <c r="AJ55" s="7"/>
-      <c r="AK55" s="7"/>
-      <c r="AL55" s="7"/>
-      <c r="AM55" s="7"/>
-      <c r="AN55" s="7"/>
-      <c r="AO55" s="7"/>
-      <c r="AP55" s="7"/>
-      <c r="AQ55" s="7"/>
-      <c r="AR55" s="7"/>
-      <c r="AS55" s="7"/>
-      <c r="AT55" s="7"/>
-      <c r="AU55" s="9"/>
+    <row r="55" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="79"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="6"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="81"/>
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+      <c r="X55" s="6"/>
+      <c r="Y55" s="6"/>
+      <c r="Z55" s="6"/>
+      <c r="AA55" s="6"/>
+      <c r="AB55" s="6"/>
+      <c r="AC55" s="6"/>
+      <c r="AD55" s="6"/>
+      <c r="AE55" s="82"/>
+      <c r="AF55" s="6"/>
+      <c r="AG55" s="6"/>
+      <c r="AH55" s="6"/>
+      <c r="AI55" s="6"/>
+      <c r="AJ55" s="6"/>
+      <c r="AK55" s="6"/>
+      <c r="AL55" s="6"/>
+      <c r="AM55" s="6"/>
+      <c r="AN55" s="6"/>
+      <c r="AO55" s="6"/>
+      <c r="AP55" s="6"/>
+      <c r="AQ55" s="6"/>
+      <c r="AR55" s="6"/>
+      <c r="AS55" s="6"/>
+      <c r="AT55" s="6"/>
+      <c r="AU55" s="33"/>
       <c r="AV55" s="14"/>
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A56" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="47"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="48"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4"/>
-      <c r="Q56" s="4"/>
-      <c r="R56" s="4"/>
-      <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
-      <c r="U56" s="4"/>
-      <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
-      <c r="X56" s="4"/>
-      <c r="Y56" s="4"/>
-      <c r="Z56" s="4"/>
-      <c r="AA56" s="4"/>
-      <c r="AB56" s="4"/>
-      <c r="AC56" s="4"/>
-      <c r="AD56" s="4"/>
-      <c r="AE56" s="4"/>
-      <c r="AF56" s="4"/>
-      <c r="AG56" s="4"/>
-      <c r="AH56" s="4"/>
-      <c r="AI56" s="4"/>
-      <c r="AJ56" s="4"/>
-      <c r="AK56" s="4"/>
-      <c r="AL56" s="4"/>
-      <c r="AM56" s="4"/>
-      <c r="AN56" s="4"/>
-      <c r="AO56" s="4"/>
-      <c r="AP56" s="4"/>
-      <c r="AQ56" s="4"/>
-      <c r="AR56" s="4"/>
-      <c r="AS56" s="4"/>
-      <c r="AT56" s="4"/>
-      <c r="AU56" s="10"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="7"/>
+      <c r="AC56" s="7"/>
+      <c r="AD56" s="7"/>
+      <c r="AE56" s="7"/>
+      <c r="AF56" s="7"/>
+      <c r="AG56" s="7"/>
+      <c r="AH56" s="7"/>
+      <c r="AI56" s="7"/>
+      <c r="AJ56" s="7"/>
+      <c r="AK56" s="7"/>
+      <c r="AL56" s="7"/>
+      <c r="AM56" s="7"/>
+      <c r="AN56" s="7"/>
+      <c r="AO56" s="7"/>
+      <c r="AP56" s="7"/>
+      <c r="AQ56" s="7"/>
+      <c r="AR56" s="7"/>
+      <c r="AS56" s="7"/>
+      <c r="AT56" s="7"/>
+      <c r="AU56" s="9"/>
       <c r="AV56" s="14"/>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A57" s="32"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="8"/>
-      <c r="S57" s="8"/>
-      <c r="T57" s="8"/>
-      <c r="U57" s="8"/>
-      <c r="V57" s="8"/>
-      <c r="W57" s="8"/>
-      <c r="X57" s="8"/>
-      <c r="Y57" s="8"/>
-      <c r="Z57" s="8"/>
-      <c r="AA57" s="8"/>
-      <c r="AB57" s="8"/>
-      <c r="AC57" s="8"/>
-      <c r="AD57" s="8"/>
-      <c r="AE57" s="8"/>
-      <c r="AF57" s="8"/>
-      <c r="AG57" s="8"/>
-      <c r="AH57" s="8"/>
-      <c r="AI57" s="8"/>
-      <c r="AJ57" s="8"/>
-      <c r="AK57" s="8"/>
-      <c r="AL57" s="8"/>
-      <c r="AM57" s="8"/>
-      <c r="AN57" s="8"/>
-      <c r="AO57" s="8"/>
-      <c r="AP57" s="8"/>
-      <c r="AQ57" s="3"/>
-      <c r="AR57" s="159"/>
-      <c r="AS57" s="159"/>
-      <c r="AT57" s="159"/>
-      <c r="AU57" s="160"/>
+      <c r="A57" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+      <c r="AB57" s="4"/>
+      <c r="AC57" s="4"/>
+      <c r="AD57" s="4"/>
+      <c r="AE57" s="4"/>
+      <c r="AF57" s="4"/>
+      <c r="AG57" s="4"/>
+      <c r="AH57" s="4"/>
+      <c r="AI57" s="4"/>
+      <c r="AJ57" s="4"/>
+      <c r="AK57" s="4"/>
+      <c r="AL57" s="4"/>
+      <c r="AM57" s="4"/>
+      <c r="AN57" s="4"/>
+      <c r="AO57" s="4"/>
+      <c r="AP57" s="4"/>
+      <c r="AQ57" s="4"/>
+      <c r="AR57" s="4"/>
+      <c r="AS57" s="4"/>
+      <c r="AT57" s="4"/>
+      <c r="AU57" s="10"/>
       <c r="AV57" s="14"/>
     </row>
-    <row r="58" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="28"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="6"/>
-      <c r="N58" s="6"/>
-      <c r="O58" s="6"/>
-      <c r="P58" s="6"/>
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
-      <c r="S58" s="6"/>
-      <c r="T58" s="6"/>
-      <c r="U58" s="6"/>
-      <c r="V58" s="6"/>
-      <c r="W58" s="6"/>
-      <c r="X58" s="6"/>
-      <c r="Y58" s="6"/>
-      <c r="Z58" s="6"/>
-      <c r="AA58" s="6"/>
-      <c r="AB58" s="6"/>
-      <c r="AC58" s="6"/>
-      <c r="AD58" s="18"/>
-      <c r="AE58" s="6"/>
-      <c r="AF58" s="6"/>
-      <c r="AG58" s="6"/>
-      <c r="AH58" s="6"/>
-      <c r="AI58" s="6"/>
-      <c r="AJ58" s="6"/>
-      <c r="AK58" s="6"/>
-      <c r="AL58" s="6"/>
-      <c r="AM58" s="6"/>
-      <c r="AN58" s="6"/>
-      <c r="AO58" s="6"/>
-      <c r="AP58" s="6"/>
-      <c r="AQ58" s="6"/>
-      <c r="AR58" s="6"/>
-      <c r="AS58" s="6"/>
-      <c r="AT58" s="6"/>
-      <c r="AU58" s="33"/>
+    <row r="58" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A58" s="32"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+      <c r="V58" s="8"/>
+      <c r="W58" s="8"/>
+      <c r="X58" s="8"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
+      <c r="AA58" s="8"/>
+      <c r="AB58" s="8"/>
+      <c r="AC58" s="8"/>
+      <c r="AD58" s="8"/>
+      <c r="AE58" s="8"/>
+      <c r="AF58" s="8"/>
+      <c r="AG58" s="8"/>
+      <c r="AH58" s="8"/>
+      <c r="AI58" s="8"/>
+      <c r="AJ58" s="8"/>
+      <c r="AK58" s="8"/>
+      <c r="AL58" s="8"/>
+      <c r="AM58" s="8"/>
+      <c r="AN58" s="8"/>
+      <c r="AO58" s="8"/>
+      <c r="AP58" s="8"/>
+      <c r="AQ58" s="3"/>
+      <c r="AR58" s="140"/>
+      <c r="AS58" s="140"/>
+      <c r="AT58" s="140"/>
+      <c r="AU58" s="141"/>
       <c r="AV58" s="14"/>
     </row>
     <row r="59" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="7"/>
-      <c r="T59" s="7"/>
-      <c r="U59" s="7"/>
-      <c r="V59" s="7"/>
-      <c r="W59" s="7"/>
-      <c r="X59" s="7"/>
-      <c r="Y59" s="7"/>
-      <c r="Z59" s="7"/>
-      <c r="AA59" s="7"/>
-      <c r="AB59" s="7"/>
-      <c r="AC59" s="7"/>
-      <c r="AD59" s="7"/>
-      <c r="AE59" s="7"/>
-      <c r="AF59" s="7"/>
-      <c r="AG59" s="7"/>
-      <c r="AH59" s="7"/>
-      <c r="AI59" s="7"/>
-      <c r="AJ59" s="7"/>
-      <c r="AK59" s="7"/>
-      <c r="AL59" s="7"/>
-      <c r="AM59" s="7"/>
-      <c r="AN59" s="7"/>
-      <c r="AO59" s="7"/>
-      <c r="AP59" s="7"/>
-      <c r="AQ59" s="7"/>
-      <c r="AR59" s="7"/>
-      <c r="AS59" s="7"/>
-      <c r="AT59" s="7"/>
-      <c r="AU59" s="9"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="6"/>
+      <c r="AA59" s="6"/>
+      <c r="AB59" s="6"/>
+      <c r="AC59" s="6"/>
+      <c r="AD59" s="18"/>
+      <c r="AE59" s="6"/>
+      <c r="AF59" s="6"/>
+      <c r="AG59" s="6"/>
+      <c r="AH59" s="6"/>
+      <c r="AI59" s="6"/>
+      <c r="AJ59" s="6"/>
+      <c r="AK59" s="6"/>
+      <c r="AL59" s="6"/>
+      <c r="AM59" s="6"/>
+      <c r="AN59" s="6"/>
+      <c r="AO59" s="6"/>
+      <c r="AP59" s="6"/>
+      <c r="AQ59" s="6"/>
+      <c r="AR59" s="6"/>
+      <c r="AS59" s="6"/>
+      <c r="AT59" s="6"/>
+      <c r="AU59" s="33"/>
       <c r="AV59" s="14"/>
     </row>
-    <row r="60" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="122" t="s">
-        <v>41</v>
+    <row r="60" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="30"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7"/>
+      <c r="V60" s="7"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="7"/>
+      <c r="Y60" s="7"/>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="7"/>
+      <c r="AB60" s="7"/>
+      <c r="AC60" s="7"/>
+      <c r="AD60" s="7"/>
+      <c r="AE60" s="7"/>
+      <c r="AF60" s="7"/>
+      <c r="AG60" s="7"/>
+      <c r="AH60" s="7"/>
+      <c r="AI60" s="7"/>
+      <c r="AJ60" s="7"/>
+      <c r="AK60" s="7"/>
+      <c r="AL60" s="7"/>
+      <c r="AM60" s="7"/>
+      <c r="AN60" s="7"/>
+      <c r="AO60" s="7"/>
+      <c r="AP60" s="7"/>
+      <c r="AQ60" s="7"/>
+      <c r="AR60" s="7"/>
+      <c r="AS60" s="7"/>
+      <c r="AT60" s="7"/>
+      <c r="AU60" s="9"/>
+      <c r="AV60" s="14"/>
+    </row>
+    <row r="61" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="155" t="s">
+        <v>39</v>
       </c>
-      <c r="B60" s="123"/>
-      <c r="C60" s="123"/>
-      <c r="D60" s="123"/>
-      <c r="E60" s="123"/>
-      <c r="F60" s="123"/>
-      <c r="G60" s="123"/>
-      <c r="H60" s="123"/>
-      <c r="I60" s="123"/>
-      <c r="J60" s="123"/>
-      <c r="K60" s="123"/>
-      <c r="L60" s="123"/>
-      <c r="M60" s="123"/>
-      <c r="N60" s="123"/>
-      <c r="O60" s="123"/>
-      <c r="P60" s="123"/>
-      <c r="Q60" s="123"/>
-      <c r="R60" s="123"/>
-      <c r="S60" s="123"/>
-      <c r="T60" s="123"/>
-      <c r="U60" s="123"/>
-      <c r="V60" s="123"/>
-      <c r="W60" s="123"/>
-      <c r="X60" s="123"/>
-      <c r="Y60" s="123"/>
-      <c r="Z60" s="123"/>
-      <c r="AA60" s="123"/>
-      <c r="AB60" s="123"/>
-      <c r="AC60" s="123"/>
-      <c r="AD60" s="123"/>
-      <c r="AE60" s="123"/>
-      <c r="AF60" s="123"/>
-      <c r="AG60" s="123"/>
-      <c r="AH60" s="123"/>
-      <c r="AI60" s="123"/>
-      <c r="AJ60" s="123"/>
-      <c r="AK60" s="123"/>
-      <c r="AL60" s="123"/>
-      <c r="AM60" s="123"/>
-      <c r="AN60" s="123"/>
-      <c r="AO60" s="123"/>
-      <c r="AP60" s="123"/>
-      <c r="AQ60" s="123"/>
-      <c r="AR60" s="123"/>
-      <c r="AS60" s="123"/>
-      <c r="AT60" s="123"/>
-      <c r="AU60" s="124"/>
-      <c r="AV60" s="14"/>
-    </row>
-    <row r="61" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
-      <c r="Q61" s="4"/>
-      <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
-      <c r="U61" s="4"/>
-      <c r="V61" s="4"/>
-      <c r="W61" s="4"/>
-      <c r="X61" s="4"/>
-      <c r="Y61" s="4"/>
-      <c r="Z61" s="4"/>
-      <c r="AA61" s="4"/>
-      <c r="AB61" s="4"/>
-      <c r="AC61" s="4"/>
-      <c r="AD61" s="4"/>
-      <c r="AE61" s="4"/>
-      <c r="AF61" s="4"/>
-      <c r="AG61" s="4"/>
-      <c r="AH61" s="4"/>
-      <c r="AI61" s="4"/>
-      <c r="AJ61" s="4"/>
-      <c r="AK61" s="4"/>
-      <c r="AL61" s="4"/>
-      <c r="AM61" s="4"/>
-      <c r="AN61" s="4"/>
-      <c r="AO61" s="4"/>
-      <c r="AP61" s="4"/>
-      <c r="AQ61" s="4"/>
-      <c r="AR61" s="4"/>
-      <c r="AS61" s="4"/>
-      <c r="AT61" s="4"/>
-      <c r="AU61" s="10"/>
+      <c r="B61" s="156"/>
+      <c r="C61" s="156"/>
+      <c r="D61" s="156"/>
+      <c r="E61" s="156"/>
+      <c r="F61" s="156"/>
+      <c r="G61" s="156"/>
+      <c r="H61" s="156"/>
+      <c r="I61" s="156"/>
+      <c r="J61" s="156"/>
+      <c r="K61" s="156"/>
+      <c r="L61" s="156"/>
+      <c r="M61" s="156"/>
+      <c r="N61" s="156"/>
+      <c r="O61" s="156"/>
+      <c r="P61" s="156"/>
+      <c r="Q61" s="156"/>
+      <c r="R61" s="156"/>
+      <c r="S61" s="156"/>
+      <c r="T61" s="156"/>
+      <c r="U61" s="156"/>
+      <c r="V61" s="156"/>
+      <c r="W61" s="156"/>
+      <c r="X61" s="156"/>
+      <c r="Y61" s="156"/>
+      <c r="Z61" s="156"/>
+      <c r="AA61" s="156"/>
+      <c r="AB61" s="156"/>
+      <c r="AC61" s="156"/>
+      <c r="AD61" s="156"/>
+      <c r="AE61" s="156"/>
+      <c r="AF61" s="156"/>
+      <c r="AG61" s="156"/>
+      <c r="AH61" s="156"/>
+      <c r="AI61" s="156"/>
+      <c r="AJ61" s="156"/>
+      <c r="AK61" s="156"/>
+      <c r="AL61" s="156"/>
+      <c r="AM61" s="156"/>
+      <c r="AN61" s="156"/>
+      <c r="AO61" s="156"/>
+      <c r="AP61" s="156"/>
+      <c r="AQ61" s="156"/>
+      <c r="AR61" s="156"/>
+      <c r="AS61" s="156"/>
+      <c r="AT61" s="156"/>
+      <c r="AU61" s="157"/>
       <c r="AV61" s="14"/>
     </row>
-    <row r="62" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A62" s="161" t="s">
+    <row r="62" spans="1:48" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="34"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
+      <c r="X62" s="4"/>
+      <c r="Y62" s="4"/>
+      <c r="Z62" s="4"/>
+      <c r="AA62" s="4"/>
+      <c r="AB62" s="4"/>
+      <c r="AC62" s="4"/>
+      <c r="AD62" s="4"/>
+      <c r="AE62" s="4"/>
+      <c r="AF62" s="4"/>
+      <c r="AG62" s="4"/>
+      <c r="AH62" s="4"/>
+      <c r="AI62" s="4"/>
+      <c r="AJ62" s="4"/>
+      <c r="AK62" s="4"/>
+      <c r="AL62" s="4"/>
+      <c r="AM62" s="4"/>
+      <c r="AN62" s="4"/>
+      <c r="AO62" s="4"/>
+      <c r="AP62" s="4"/>
+      <c r="AQ62" s="4"/>
+      <c r="AR62" s="4"/>
+      <c r="AS62" s="4"/>
+      <c r="AT62" s="4"/>
+      <c r="AU62" s="10"/>
+      <c r="AV62" s="14"/>
+    </row>
+    <row r="63" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A63" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="162"/>
-      <c r="C62" s="162"/>
-      <c r="D62" s="162"/>
-      <c r="E62" s="162"/>
-      <c r="F62" s="162"/>
-      <c r="G62" s="162"/>
-      <c r="H62" s="162"/>
-      <c r="I62" s="162"/>
-      <c r="J62" s="162"/>
-      <c r="K62" s="162"/>
-      <c r="L62" s="162"/>
-      <c r="M62" s="162"/>
-      <c r="N62" s="162"/>
-      <c r="O62" s="162"/>
-      <c r="P62" s="162"/>
-      <c r="Q62" s="162"/>
-      <c r="R62" s="162"/>
-      <c r="S62" s="162"/>
-      <c r="T62" s="162"/>
-      <c r="U62" s="162"/>
-      <c r="V62" s="162"/>
-      <c r="W62" s="162"/>
-      <c r="X62" s="162"/>
-      <c r="Y62" s="163"/>
-      <c r="Z62" s="161" t="s">
+      <c r="B63" s="142"/>
+      <c r="C63" s="142"/>
+      <c r="D63" s="142"/>
+      <c r="E63" s="142"/>
+      <c r="F63" s="142"/>
+      <c r="G63" s="142"/>
+      <c r="H63" s="142"/>
+      <c r="I63" s="142"/>
+      <c r="J63" s="142"/>
+      <c r="K63" s="142"/>
+      <c r="L63" s="142"/>
+      <c r="M63" s="142"/>
+      <c r="N63" s="142"/>
+      <c r="O63" s="142"/>
+      <c r="P63" s="142"/>
+      <c r="Q63" s="142"/>
+      <c r="R63" s="142"/>
+      <c r="S63" s="142"/>
+      <c r="T63" s="142"/>
+      <c r="U63" s="142"/>
+      <c r="V63" s="142"/>
+      <c r="W63" s="142"/>
+      <c r="X63" s="142"/>
+      <c r="Y63" s="135"/>
+      <c r="Z63" s="134" t="s">
         <v>27</v>
       </c>
-      <c r="AA62" s="162"/>
-      <c r="AB62" s="162"/>
-      <c r="AC62" s="162"/>
-      <c r="AD62" s="162"/>
-      <c r="AE62" s="162"/>
-      <c r="AF62" s="162"/>
-      <c r="AG62" s="162"/>
-      <c r="AH62" s="162"/>
-      <c r="AI62" s="162"/>
-      <c r="AJ62" s="162"/>
-      <c r="AK62" s="162"/>
-      <c r="AL62" s="162"/>
-      <c r="AM62" s="162"/>
-      <c r="AN62" s="162"/>
-      <c r="AO62" s="162"/>
-      <c r="AP62" s="162"/>
-      <c r="AQ62" s="162"/>
-      <c r="AR62" s="162"/>
-      <c r="AS62" s="162"/>
-      <c r="AT62" s="162"/>
-      <c r="AU62" s="163"/>
-      <c r="AV62" s="14"/>
-    </row>
-    <row r="63" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
-      <c r="U63" s="4"/>
-      <c r="V63" s="4"/>
-      <c r="W63" s="4"/>
-      <c r="X63" s="4"/>
-      <c r="Y63" s="4"/>
-      <c r="Z63" s="14"/>
-      <c r="AA63" s="4"/>
-      <c r="AB63" s="4"/>
-      <c r="AC63" s="4"/>
-      <c r="AD63" s="4"/>
-      <c r="AE63" s="4"/>
-      <c r="AF63" s="4"/>
-      <c r="AG63" s="4"/>
-      <c r="AH63" s="4"/>
-      <c r="AI63" s="4"/>
-      <c r="AJ63" s="4"/>
-      <c r="AK63" s="4"/>
-      <c r="AL63" s="4"/>
-      <c r="AM63" s="4"/>
-      <c r="AN63" s="4"/>
-      <c r="AO63" s="4"/>
-      <c r="AP63" s="4"/>
-      <c r="AQ63" s="4"/>
-      <c r="AR63" s="4"/>
-      <c r="AS63" s="4"/>
-      <c r="AT63" s="4"/>
-      <c r="AU63" s="10"/>
+      <c r="AA63" s="142"/>
+      <c r="AB63" s="142"/>
+      <c r="AC63" s="142"/>
+      <c r="AD63" s="142"/>
+      <c r="AE63" s="142"/>
+      <c r="AF63" s="142"/>
+      <c r="AG63" s="142"/>
+      <c r="AH63" s="142"/>
+      <c r="AI63" s="142"/>
+      <c r="AJ63" s="142"/>
+      <c r="AK63" s="142"/>
+      <c r="AL63" s="142"/>
+      <c r="AM63" s="142"/>
+      <c r="AN63" s="142"/>
+      <c r="AO63" s="142"/>
+      <c r="AP63" s="142"/>
+      <c r="AQ63" s="142"/>
+      <c r="AR63" s="142"/>
+      <c r="AS63" s="142"/>
+      <c r="AT63" s="142"/>
+      <c r="AU63" s="135"/>
       <c r="AV63" s="14"/>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.2">
@@ -4950,9 +4983,9 @@
       <c r="A71" s="14"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="2"/>
+      <c r="D71" s="4"/>
       <c r="E71" s="4"/>
-      <c r="F71" s="2"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -4979,122 +5012,151 @@
       <c r="AD71" s="4"/>
       <c r="AE71" s="4"/>
       <c r="AF71" s="4"/>
-      <c r="AG71" s="2"/>
+      <c r="AG71" s="4"/>
       <c r="AH71" s="4"/>
       <c r="AI71" s="4"/>
-      <c r="AJ71" s="158"/>
-      <c r="AK71" s="158"/>
-      <c r="AL71" s="158"/>
-      <c r="AM71" s="158"/>
-      <c r="AN71" s="158"/>
-      <c r="AO71" s="158"/>
-      <c r="AP71" s="158"/>
-      <c r="AQ71" s="158"/>
-      <c r="AR71" s="158"/>
-      <c r="AS71" s="158"/>
+      <c r="AJ71" s="4"/>
+      <c r="AK71" s="4"/>
+      <c r="AL71" s="4"/>
+      <c r="AM71" s="4"/>
+      <c r="AN71" s="4"/>
+      <c r="AO71" s="4"/>
+      <c r="AP71" s="4"/>
+      <c r="AQ71" s="4"/>
+      <c r="AR71" s="4"/>
+      <c r="AS71" s="4"/>
       <c r="AT71" s="4"/>
       <c r="AU71" s="10"/>
       <c r="AV71" s="14"/>
     </row>
     <row r="72" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A72" s="13"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-      <c r="M72" s="8"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="8"/>
-      <c r="S72" s="8"/>
-      <c r="T72" s="8"/>
-      <c r="U72" s="8"/>
-      <c r="V72" s="8"/>
-      <c r="W72" s="8"/>
-      <c r="X72" s="8"/>
-      <c r="Y72" s="8"/>
-      <c r="Z72" s="13"/>
-      <c r="AA72" s="8"/>
-      <c r="AB72" s="8"/>
-      <c r="AC72" s="8"/>
-      <c r="AD72" s="8"/>
-      <c r="AE72" s="8"/>
-      <c r="AF72" s="8"/>
-      <c r="AG72" s="3"/>
-      <c r="AH72" s="8"/>
-      <c r="AI72" s="8"/>
-      <c r="AJ72" s="8"/>
-      <c r="AK72" s="8"/>
-      <c r="AL72" s="49"/>
-      <c r="AM72" s="8"/>
-      <c r="AN72" s="8"/>
-      <c r="AO72" s="8"/>
-      <c r="AP72" s="8"/>
-      <c r="AQ72" s="8"/>
-      <c r="AR72" s="8"/>
-      <c r="AS72" s="8"/>
-      <c r="AT72" s="8"/>
-      <c r="AU72" s="11"/>
+      <c r="A72" s="14"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="4"/>
+      <c r="W72" s="4"/>
+      <c r="X72" s="4"/>
+      <c r="Y72" s="4"/>
+      <c r="Z72" s="14"/>
+      <c r="AA72" s="4"/>
+      <c r="AB72" s="4"/>
+      <c r="AC72" s="4"/>
+      <c r="AD72" s="4"/>
+      <c r="AE72" s="4"/>
+      <c r="AF72" s="4"/>
+      <c r="AG72" s="2"/>
+      <c r="AH72" s="4"/>
+      <c r="AI72" s="4"/>
+      <c r="AJ72" s="139"/>
+      <c r="AK72" s="139"/>
+      <c r="AL72" s="139"/>
+      <c r="AM72" s="139"/>
+      <c r="AN72" s="139"/>
+      <c r="AO72" s="139"/>
+      <c r="AP72" s="139"/>
+      <c r="AQ72" s="139"/>
+      <c r="AR72" s="139"/>
+      <c r="AS72" s="139"/>
+      <c r="AT72" s="4"/>
+      <c r="AU72" s="10"/>
       <c r="AV72" s="14"/>
     </row>
     <row r="73" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="B73" s="1"/>
-      <c r="N73" s="1"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="8"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="8"/>
+      <c r="R73" s="8"/>
+      <c r="S73" s="8"/>
+      <c r="T73" s="8"/>
+      <c r="U73" s="8"/>
+      <c r="V73" s="8"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="13"/>
+      <c r="AA73" s="8"/>
+      <c r="AB73" s="8"/>
+      <c r="AC73" s="8"/>
+      <c r="AD73" s="8"/>
+      <c r="AE73" s="8"/>
+      <c r="AF73" s="8"/>
+      <c r="AG73" s="3"/>
+      <c r="AH73" s="8"/>
+      <c r="AI73" s="8"/>
+      <c r="AJ73" s="8"/>
+      <c r="AK73" s="8"/>
+      <c r="AL73" s="49"/>
+      <c r="AM73" s="8"/>
+      <c r="AN73" s="8"/>
+      <c r="AO73" s="8"/>
+      <c r="AP73" s="8"/>
+      <c r="AQ73" s="8"/>
+      <c r="AR73" s="8"/>
+      <c r="AS73" s="8"/>
+      <c r="AT73" s="8"/>
+      <c r="AU73" s="11"/>
+      <c r="AV73" s="14"/>
+    </row>
+    <row r="74" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B74" s="1"/>
+      <c r="N74" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="Z36:AD36"/>
-    <mergeCell ref="Z37:AD37"/>
-    <mergeCell ref="Z40:AD40"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="Z38:AD38"/>
-    <mergeCell ref="Z32:AD32"/>
-    <mergeCell ref="Z33:AD33"/>
-    <mergeCell ref="Z34:AD34"/>
-    <mergeCell ref="Z35:AD35"/>
-    <mergeCell ref="Z39:AD39"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A29:B30"/>
+  <mergeCells count="79">
+    <mergeCell ref="AL12:AT12"/>
+    <mergeCell ref="AO27:AT27"/>
+    <mergeCell ref="AF36:AM36"/>
+    <mergeCell ref="AF37:AM37"/>
+    <mergeCell ref="AF38:AM38"/>
     <mergeCell ref="AF32:AM32"/>
     <mergeCell ref="AF33:AM33"/>
     <mergeCell ref="AF34:AM34"/>
-    <mergeCell ref="AF35:AM35"/>
-    <mergeCell ref="Y29:AE30"/>
-    <mergeCell ref="C29:X30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="Z31:AD31"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AM6:AS6"/>
-    <mergeCell ref="AJ71:AS71"/>
-    <mergeCell ref="AR57:AU57"/>
-    <mergeCell ref="Z62:AU62"/>
-    <mergeCell ref="Y45:Z45"/>
-    <mergeCell ref="AJ24:AM25"/>
-    <mergeCell ref="AF24:AI25"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="AF28:AI28"/>
-    <mergeCell ref="A62:Y62"/>
-    <mergeCell ref="A10:AU10"/>
-    <mergeCell ref="A17:AU17"/>
-    <mergeCell ref="A60:AU60"/>
-    <mergeCell ref="AN24:AU25"/>
-    <mergeCell ref="AN27:AU27"/>
+    <mergeCell ref="AN53:AO53"/>
+    <mergeCell ref="AP53:AU53"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="N22:Y22"/>
+    <mergeCell ref="Z22:AG22"/>
+    <mergeCell ref="A44:AU44"/>
+    <mergeCell ref="C24:AE25"/>
+    <mergeCell ref="AN26:AU26"/>
+    <mergeCell ref="AN28:AU28"/>
+    <mergeCell ref="AN29:AU30"/>
+    <mergeCell ref="AF29:AM30"/>
+    <mergeCell ref="AF31:AM31"/>
+    <mergeCell ref="AF41:AM41"/>
+    <mergeCell ref="AF39:AM39"/>
     <mergeCell ref="A24:B25"/>
     <mergeCell ref="Y13:AE13"/>
     <mergeCell ref="AJ27:AM27"/>
@@ -5102,33 +5164,56 @@
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="L15:AT15"/>
     <mergeCell ref="AL13:AT13"/>
-    <mergeCell ref="AN52:AO52"/>
-    <mergeCell ref="AP52:AU52"/>
-    <mergeCell ref="A22:M22"/>
-    <mergeCell ref="N22:Y22"/>
-    <mergeCell ref="Z22:AG22"/>
-    <mergeCell ref="A43:AU43"/>
-    <mergeCell ref="C24:AE25"/>
-    <mergeCell ref="AN26:AU26"/>
-    <mergeCell ref="AN28:AU28"/>
-    <mergeCell ref="AN29:AU30"/>
-    <mergeCell ref="AF29:AM30"/>
-    <mergeCell ref="AF31:AM31"/>
-    <mergeCell ref="AF40:AM40"/>
-    <mergeCell ref="AO31:AT31"/>
-    <mergeCell ref="AO32:AT32"/>
-    <mergeCell ref="AO33:AT33"/>
-    <mergeCell ref="AO40:AT40"/>
-    <mergeCell ref="AF36:AM36"/>
-    <mergeCell ref="AF37:AM37"/>
-    <mergeCell ref="AO34:AT34"/>
-    <mergeCell ref="AO35:AT35"/>
-    <mergeCell ref="AO36:AT36"/>
-    <mergeCell ref="AO37:AT37"/>
-    <mergeCell ref="AO38:AT38"/>
-    <mergeCell ref="AO39:AT39"/>
-    <mergeCell ref="AF38:AM38"/>
-    <mergeCell ref="AF39:AM39"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AM6:AS6"/>
+    <mergeCell ref="AJ72:AS72"/>
+    <mergeCell ref="AR58:AU58"/>
+    <mergeCell ref="Z63:AU63"/>
+    <mergeCell ref="Y46:Z46"/>
+    <mergeCell ref="AJ24:AM25"/>
+    <mergeCell ref="AF24:AI25"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="A63:Y63"/>
+    <mergeCell ref="A10:AU10"/>
+    <mergeCell ref="A17:AU17"/>
+    <mergeCell ref="A61:AU61"/>
+    <mergeCell ref="AN24:AU25"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="AF35:AM35"/>
+    <mergeCell ref="Y29:AE30"/>
+    <mergeCell ref="C29:X30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="Z31:AD31"/>
+    <mergeCell ref="Z32:AD32"/>
+    <mergeCell ref="Z33:AD33"/>
+    <mergeCell ref="Z34:AD34"/>
+    <mergeCell ref="Z35:AD35"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="Z36:AD36"/>
+    <mergeCell ref="Z37:AD37"/>
+    <mergeCell ref="Z41:AD41"/>
+    <mergeCell ref="Z38:AD38"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="Z39:AD39"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="AP41:AT41"/>
+    <mergeCell ref="AP32:AT32"/>
+    <mergeCell ref="AP33:AT33"/>
+    <mergeCell ref="AP34:AT34"/>
+    <mergeCell ref="AP35:AT35"/>
+    <mergeCell ref="AP36:AT36"/>
+    <mergeCell ref="AP31:AT31"/>
+    <mergeCell ref="AP37:AT37"/>
+    <mergeCell ref="AP38:AT38"/>
+    <mergeCell ref="AP39:AT39"/>
+    <mergeCell ref="AP40:AT40"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.51181102362204722" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>